<commit_message>
Add VC 6.0 to IDEA map table to readme. Edited XLSX tracker.
</commit_message>
<xml_diff>
--- a/WellEngineered.us VC++ 6.0 Shortcuts.xlsx
+++ b/WellEngineered.us VC++ 6.0 Shortcuts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB1EEDF-B862-4D08-A451-2049AC65D127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B3E717-587A-4343-98E7-A2B47D99A69F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5D8658FC-F053-4B4D-BC9B-4C701ADA3E99}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1496">
   <si>
     <t>Shortcut keys</t>
   </si>
@@ -4691,6 +4691,9 @@
   <si>
     <t>CollapseAll
 ExpandAll</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -4749,7 +4752,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -4767,21 +4773,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C02C956-582F-44C3-AEF8-8DB3931088CF}" name="Table1" displayName="Table1" ref="A1:G204" totalsRowShown="0">
-  <autoFilter ref="A1:G204" xr:uid="{845A4353-964A-4DBA-9B4F-B53FE6686E31}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G204">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C02C956-582F-44C3-AEF8-8DB3931088CF}" name="Table1" displayName="Table1" ref="A1:H204" totalsRowShown="0">
+  <autoFilter ref="A1:H204" xr:uid="{845A4353-964A-4DBA-9B4F-B53FE6686E31}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H204">
     <sortCondition ref="A2:A204"/>
     <sortCondition ref="B2:B204"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="5" xr3:uid="{5F34C1A2-157F-413E-9C0B-7C76A830218E}" name="VC_Command_Class"/>
     <tableColumn id="1" xr3:uid="{B2DDF3DF-1DA0-4339-9484-726734A517D3}" name="VC_Command_Name"/>
     <tableColumn id="2" xr3:uid="{EC6985FC-BD16-4E9B-AAF1-A13EABDAD49B}" name="Shortcut keys"/>
     <tableColumn id="4" xr3:uid="{25DFAA24-6FA3-4E65-A8ED-B79BE5D14C86}" name="VC_Shortcut_Keys"/>
-    <tableColumn id="6" xr3:uid="{0093AADA-341A-4714-8E9D-194CA52EE50D}" name="VC_SK_X" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{0093AADA-341A-4714-8E9D-194CA52EE50D}" name="VC_SK_X" dataDxfId="1">
       <calculatedColumnFormula>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{AD3AB443-69FC-4ED6-9DE9-F3E9E01AD994}" name="IDEA_Keymap_ID"/>
+    <tableColumn id="8" xr3:uid="{9C6E70BC-6004-42BB-8E99-008FFF3A215B}" name="Column1" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="3" xr3:uid="{4EBEDB49-82CC-456A-8155-4D2F3CD27D4E}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5085,11 +5094,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D07097-255A-46B5-AC8C-91A030E6460F}">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5098,11 +5105,12 @@
     <col min="4" max="4" width="49.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="222.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="222.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="122" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>825</v>
       </c>
@@ -5122,10 +5130,13 @@
         <v>621</v>
       </c>
       <c r="G1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>249</v>
       </c>
@@ -5145,11 +5156,15 @@
       <c r="F2" t="s">
         <v>1178</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.ApplyCodeChanges|N/A</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>249</v>
       </c>
@@ -5169,11 +5184,15 @@
       <c r="F3" t="s">
         <v>1178</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Autos|N/A</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>249</v>
       </c>
@@ -5193,11 +5212,15 @@
       <c r="F4" t="s">
         <v>871</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.BreakAll|Pause</v>
+      </c>
+      <c r="H4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>249</v>
       </c>
@@ -5217,11 +5240,15 @@
       <c r="F5" t="s">
         <v>837</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Breakpoints|ViewBreakpoints</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>249</v>
       </c>
@@ -5241,11 +5268,15 @@
       <c r="F6" t="s">
         <v>1178</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.CallStack|N/A</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -5265,11 +5296,15 @@
       <c r="F7" t="s">
         <v>1040</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.ClearAllBreakpoints|RiderRemoveAllLineBreakpoints</v>
+      </c>
+      <c r="H7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -5289,9 +5324,13 @@
       <c r="F8" t="s">
         <v>851</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Continue ***|Resume</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>249</v>
       </c>
@@ -5311,11 +5350,15 @@
       <c r="F9" t="s">
         <v>858</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Disassembly|ActivateILViewerToolWindow</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>249</v>
       </c>
@@ -5335,11 +5378,15 @@
       <c r="F10" t="s">
         <v>853</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.EnableBreakpoint|ToggleBreakpointEnabled</v>
+      </c>
+      <c r="H10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>249</v>
       </c>
@@ -5359,11 +5406,15 @@
       <c r="F11" t="s">
         <v>1490</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Exceptions|OpenExceptionSettings</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -5383,11 +5434,15 @@
       <c r="F12" t="s">
         <v>1491</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Immediate|NavigateToImmediateWindow</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>249</v>
       </c>
@@ -5407,11 +5462,15 @@
       <c r="F13" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Locals|N/A</v>
+      </c>
+      <c r="H13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>249</v>
       </c>
@@ -5431,11 +5490,15 @@
       <c r="F14" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Memory1|N/A</v>
+      </c>
+      <c r="H14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>249</v>
       </c>
@@ -5455,11 +5518,15 @@
       <c r="F15" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Memory2|N/A</v>
+      </c>
+      <c r="H15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>249</v>
       </c>
@@ -5479,11 +5546,15 @@
       <c r="F16" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Memory3|N/A</v>
+      </c>
+      <c r="H16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>249</v>
       </c>
@@ -5503,11 +5574,15 @@
       <c r="F17" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Memory4|N/A</v>
+      </c>
+      <c r="H17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>249</v>
       </c>
@@ -5527,11 +5602,15 @@
       <c r="F18" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Modules|N/A</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>249</v>
       </c>
@@ -5551,11 +5630,15 @@
       <c r="F19" t="s">
         <v>855</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.NewBreakpoint|ToggleTemporaryLineBreakpoint</v>
+      </c>
+      <c r="H19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>249</v>
       </c>
@@ -5575,11 +5658,15 @@
       <c r="F20" t="s">
         <v>1178</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.QuickWatch|N/A</v>
+      </c>
+      <c r="H20" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>249</v>
       </c>
@@ -5599,11 +5686,15 @@
       <c r="F21" t="s">
         <v>1178</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Registers|N/A</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>249</v>
       </c>
@@ -5623,11 +5714,15 @@
       <c r="F22" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Restart|N/A</v>
+      </c>
+      <c r="H22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>249</v>
       </c>
@@ -5647,11 +5742,15 @@
       <c r="F23" t="s">
         <v>1178</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.RunningDocuments|N/A</v>
+      </c>
+      <c r="H23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>249</v>
       </c>
@@ -5671,11 +5770,15 @@
       <c r="F24" t="s">
         <v>857</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.RunToCursor|RunToCursor</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>249</v>
       </c>
@@ -5695,11 +5798,15 @@
       <c r="F25" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="2" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.SetNextStatement|N/A</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>249</v>
       </c>
@@ -5719,11 +5826,15 @@
       <c r="F26" t="s">
         <v>854</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.ShowNextStatement|ShowExecutionPoint</v>
+      </c>
+      <c r="H26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>249</v>
       </c>
@@ -5743,11 +5854,15 @@
       <c r="F27" t="s">
         <v>872</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Start (Continue)|#</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>249</v>
       </c>
@@ -5767,9 +5882,13 @@
       <c r="F28" t="s">
         <v>850</v>
       </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G28" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Start ***|Debug</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>249</v>
       </c>
@@ -5789,11 +5908,15 @@
       <c r="F29" t="s">
         <v>856</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.StartWithoutDebugging|Run</v>
+      </c>
+      <c r="H29" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>249</v>
       </c>
@@ -5813,11 +5936,15 @@
       <c r="F30" t="s">
         <v>859</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.StepInto|StepInto</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>249</v>
       </c>
@@ -5837,11 +5964,15 @@
       <c r="F31" t="s">
         <v>860</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.StepOut|StepOut</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>249</v>
       </c>
@@ -5861,11 +5992,15 @@
       <c r="F32" t="s">
         <v>861</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.StepOver|StepOver</v>
+      </c>
+      <c r="H32" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>249</v>
       </c>
@@ -5885,11 +6020,15 @@
       <c r="F33" t="s">
         <v>862</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.StopDebugging|Stop</v>
+      </c>
+      <c r="H33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>249</v>
       </c>
@@ -5909,11 +6048,15 @@
       <c r="F34" t="s">
         <v>1178</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.This|N/A</v>
+      </c>
+      <c r="H34" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>249</v>
       </c>
@@ -5933,11 +6076,15 @@
       <c r="F35" t="s">
         <v>1178</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.Threads|N/A</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>249</v>
       </c>
@@ -5957,11 +6104,15 @@
       <c r="F36" t="s">
         <v>852</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.ToggleBreakpoint|ToggleLineBreakpoint</v>
+      </c>
+      <c r="H36" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>249</v>
       </c>
@@ -5981,11 +6132,15 @@
       <c r="F37" t="s">
         <v>1178</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Debug.ToggleDisassembly|N/A</v>
+      </c>
+      <c r="H37" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>249</v>
       </c>
@@ -6005,11 +6160,15 @@
       <c r="F38" t="s">
         <v>836</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Debug Shortcut Keys|Tools.DebugProcesses|XDebugger.AttachToProcess</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>248</v>
       </c>
@@ -6029,11 +6188,15 @@
       <c r="F39" t="s">
         <v>622</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.Copy|$Copy</v>
+      </c>
+      <c r="H39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>248</v>
       </c>
@@ -6053,11 +6216,15 @@
       <c r="F40" t="s">
         <v>623</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.Cut|$Cut</v>
+      </c>
+      <c r="H40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>248</v>
       </c>
@@ -6077,11 +6244,15 @@
       <c r="F41" t="s">
         <v>1178</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.CycleClipboardRing|N/A</v>
+      </c>
+      <c r="H41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>248</v>
       </c>
@@ -6101,11 +6272,15 @@
       <c r="F42" t="s">
         <v>1181</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.GotoNextLocation|GotoNextError</v>
+      </c>
+      <c r="H42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>248</v>
       </c>
@@ -6125,11 +6300,15 @@
       <c r="F43" t="s">
         <v>1182</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.GotoPreviousLocation|GotoPreviousError</v>
+      </c>
+      <c r="H43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>248</v>
       </c>
@@ -6146,11 +6325,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.GoToReference|</v>
+      </c>
+      <c r="H44" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>248</v>
       </c>
@@ -6167,11 +6350,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.ListMembers|</v>
+      </c>
+      <c r="H45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>248</v>
       </c>
@@ -6191,11 +6378,15 @@
       <c r="F46" t="s">
         <v>624</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.Paste|$Paste</v>
+      </c>
+      <c r="H46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>248</v>
       </c>
@@ -6215,11 +6406,15 @@
       <c r="F47" t="s">
         <v>625</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.Redo|$Redo</v>
+      </c>
+      <c r="H47" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>248</v>
       </c>
@@ -6239,11 +6434,15 @@
       <c r="F48" t="s">
         <v>637</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.SelectionCancel|EditorEscape</v>
+      </c>
+      <c r="H48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>248</v>
       </c>
@@ -6263,11 +6462,15 @@
       <c r="F49" t="s">
         <v>626</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Edit.Undo|$Undo</v>
+      </c>
+      <c r="H49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>248</v>
       </c>
@@ -6287,11 +6490,15 @@
       <c r="F50" t="s">
         <v>838</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|File.Print|Print</v>
+      </c>
+      <c r="H50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>248</v>
       </c>
@@ -6311,11 +6518,15 @@
       <c r="F51" t="s">
         <v>835</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|File.SaveAll|SaveAll</v>
+      </c>
+      <c r="H51" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>248</v>
       </c>
@@ -6335,11 +6546,15 @@
       <c r="F52" t="s">
         <v>839</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|File.SaveSelectedItems|SaveDocument</v>
+      </c>
+      <c r="H52" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>248</v>
       </c>
@@ -6359,11 +6574,15 @@
       <c r="F53" t="s">
         <v>1178</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|Tools.GoToCommandLine|N/A</v>
+      </c>
+      <c r="H53" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>248</v>
       </c>
@@ -6380,11 +6599,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.NextTask|</v>
+      </c>
+      <c r="H54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>248</v>
       </c>
@@ -6401,11 +6624,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.PopBrowseContext|</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>248</v>
       </c>
@@ -6422,11 +6649,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.PreviousTask|</v>
+      </c>
+      <c r="H56" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -6446,11 +6677,15 @@
       <c r="F57" t="s">
         <v>1178</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.ViewCode|N/A</v>
+      </c>
+      <c r="H57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -6470,11 +6705,15 @@
       <c r="F58" t="s">
         <v>1178</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.ViewDesigner|N/A</v>
+      </c>
+      <c r="H58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>248</v>
       </c>
@@ -6494,11 +6733,15 @@
       <c r="F59" t="s">
         <v>830</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.WebNavigateBack|Back</v>
+      </c>
+      <c r="H59" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>248</v>
       </c>
@@ -6518,11 +6761,15 @@
       <c r="F60" t="s">
         <v>831</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Global Shortcut Keys|View.WebNavigateForward|Forward</v>
+      </c>
+      <c r="H60" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>273</v>
       </c>
@@ -6542,11 +6789,15 @@
       <c r="F61" t="s">
         <v>1338</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|Edit.FindSymbol|GotoSymbol</v>
+      </c>
+      <c r="H61" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>273</v>
       </c>
@@ -6563,11 +6814,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|Edit.GoToDeclaration|</v>
+      </c>
+      <c r="H62" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>273</v>
       </c>
@@ -6587,11 +6842,15 @@
       <c r="F63" t="s">
         <v>1180</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|Edit.GoToDefinition|GotoDeclaration</v>
+      </c>
+      <c r="H63" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>273</v>
       </c>
@@ -6608,11 +6867,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|View.FindSymbolResults|</v>
+      </c>
+      <c r="H64" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>273</v>
       </c>
@@ -6632,11 +6895,15 @@
       <c r="F65" t="s">
         <v>1178</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|View.ObjectBrowser|N/A</v>
+      </c>
+      <c r="H65" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>273</v>
       </c>
@@ -6656,11 +6923,15 @@
       <c r="F66" t="s">
         <v>1178</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|View.ObjectBrowserBack|N/A</v>
+      </c>
+      <c r="H66" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>273</v>
       </c>
@@ -6677,11 +6948,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Object Browser Shortcut Keys|View.ObjectBrowserForward|</v>
+      </c>
+      <c r="H67" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>250</v>
       </c>
@@ -6701,11 +6976,15 @@
       <c r="F68" t="s">
         <v>865</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|Build.BuildSolution|BuildSolutionAction</v>
+      </c>
+      <c r="H68" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>250</v>
       </c>
@@ -6725,11 +7004,15 @@
       <c r="F69" t="s">
         <v>866</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|Build.Cancel|CancelBuildAction</v>
+      </c>
+      <c r="H69" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>250</v>
       </c>
@@ -6749,11 +7032,15 @@
       <c r="F70" t="s">
         <v>867</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|Build.Compile|RebuildSolutionAction</v>
+      </c>
+      <c r="H70" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>250</v>
       </c>
@@ -6770,11 +7057,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|File.AddExistingItem|</v>
+      </c>
+      <c r="H71" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>250</v>
       </c>
@@ -6791,11 +7082,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|File.AddNewItem|</v>
+      </c>
+      <c r="H72" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>250</v>
       </c>
@@ -6815,11 +7110,15 @@
       <c r="F73" t="s">
         <v>869</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|File.NewFile|NewElement</v>
+      </c>
+      <c r="H73" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>250</v>
       </c>
@@ -6839,11 +7138,15 @@
       <c r="F74" t="s">
         <v>989</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|File.NewProject|NewProject</v>
+      </c>
+      <c r="H74" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>250</v>
       </c>
@@ -6863,11 +7166,15 @@
       <c r="F75" t="s">
         <v>870</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|File.OpenFile|OpenFile</v>
+      </c>
+      <c r="H75" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>250</v>
       </c>
@@ -6887,11 +7194,15 @@
       <c r="F76" t="s">
         <v>1039</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|File.OpenProject|RiderOpenSolution</v>
+      </c>
+      <c r="H76" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>250</v>
       </c>
@@ -6911,11 +7222,15 @@
       <c r="F77" t="s">
         <v>868</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Project Shortcut Keys|Project.Override|OverrideMethods</v>
+      </c>
+      <c r="H77" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>251</v>
       </c>
@@ -6935,11 +7250,15 @@
       <c r="F78" t="s">
         <v>904</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.Find|Find</v>
+      </c>
+      <c r="H78" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>251</v>
       </c>
@@ -6959,11 +7278,15 @@
       <c r="F79" t="s">
         <v>905</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.FindinFiles|FindInPath</v>
+      </c>
+      <c r="H79" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>251</v>
       </c>
@@ -6983,11 +7306,15 @@
       <c r="F80" t="s">
         <v>906</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.FindNext|FindNext</v>
+      </c>
+      <c r="H80" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>251</v>
       </c>
@@ -7004,11 +7331,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.FindNextSelected|</v>
+      </c>
+      <c r="H81" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -7028,11 +7359,15 @@
       <c r="F82" t="s">
         <v>907</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.FindPrevious|FindPrevious</v>
+      </c>
+      <c r="H82" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>251</v>
       </c>
@@ -7049,11 +7384,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.FindPreviousSelected|</v>
+      </c>
+      <c r="H83" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>251</v>
       </c>
@@ -7073,11 +7412,15 @@
       <c r="F84" t="s">
         <v>1178</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.GoToFindCombo|N/A</v>
+      </c>
+      <c r="H84" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>251</v>
       </c>
@@ -7097,11 +7440,15 @@
       <c r="F85" t="s">
         <v>1178</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.HiddenText|N/A</v>
+      </c>
+      <c r="H85" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>251</v>
       </c>
@@ -7118,11 +7465,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.IncrementalSearch|</v>
+      </c>
+      <c r="H86" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>251</v>
       </c>
@@ -7142,11 +7493,15 @@
       <c r="F87" t="s">
         <v>1178</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.MatchCase|N/A</v>
+      </c>
+      <c r="H87" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>251</v>
       </c>
@@ -7166,11 +7521,15 @@
       <c r="F88" t="s">
         <v>1178</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.RegularExpression|N/A</v>
+      </c>
+      <c r="H88" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>251</v>
       </c>
@@ -7190,11 +7549,15 @@
       <c r="F89" t="s">
         <v>912</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.Replace|Replace</v>
+      </c>
+      <c r="H89" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>251</v>
       </c>
@@ -7214,11 +7577,15 @@
       <c r="F90" t="s">
         <v>913</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.ReplaceinFiles|ReplaceInPath</v>
+      </c>
+      <c r="H90" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>251</v>
       </c>
@@ -7235,11 +7602,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.ReverseIncrementalSearch|</v>
+      </c>
+      <c r="H91" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -7259,11 +7630,15 @@
       <c r="F92" t="s">
         <v>1178</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.StopSearch|N/A</v>
+      </c>
+      <c r="H92" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>251</v>
       </c>
@@ -7283,11 +7658,15 @@
       <c r="F93" t="s">
         <v>1178</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.Up|N/A</v>
+      </c>
+      <c r="H93" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>251</v>
       </c>
@@ -7307,11 +7686,15 @@
       <c r="F94" t="s">
         <v>1178</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.WholeWord|N/A</v>
+      </c>
+      <c r="H94" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>251</v>
       </c>
@@ -7331,11 +7714,15 @@
       <c r="F95" t="s">
         <v>1178</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Search and Replace Shortcut Keys|Edit.Wildcard|N/A</v>
+      </c>
+      <c r="H95" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>376</v>
       </c>
@@ -7355,11 +7742,15 @@
       <c r="F96" t="s">
         <v>629</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.BreakLine|EditorEnter</v>
+      </c>
+      <c r="H96" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>376</v>
       </c>
@@ -7379,11 +7770,15 @@
       <c r="F97" t="s">
         <v>974</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.CharTranspose|EditorTranspose</v>
+      </c>
+      <c r="H97" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>376</v>
       </c>
@@ -7400,11 +7795,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>1</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ClearBookmarks|</v>
+      </c>
+      <c r="H98" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>376</v>
       </c>
@@ -7421,11 +7820,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>1</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.CollapsetoDefinitions|</v>
+      </c>
+      <c r="H99" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>376</v>
       </c>
@@ -7445,11 +7848,15 @@
       <c r="F100" t="s">
         <v>1219</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G100" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.CommentSelection|CommentByLineComment</v>
+      </c>
+      <c r="H100" t="s">
         <v>1493</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>376</v>
       </c>
@@ -7469,11 +7876,15 @@
       <c r="F101" t="s">
         <v>879</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G101" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.CompleteWord|CodeCompletion</v>
+      </c>
+      <c r="H101" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>376</v>
       </c>
@@ -7493,11 +7904,15 @@
       <c r="F102" t="s">
         <v>603</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.Delete|$Delete</v>
+      </c>
+      <c r="H102" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>376</v>
       </c>
@@ -7517,11 +7932,15 @@
       <c r="F103" t="s">
         <v>632</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G103" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.DeleteBackwards|EditorBackSpace</v>
+      </c>
+      <c r="H103" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>376</v>
       </c>
@@ -7541,11 +7960,15 @@
       <c r="F104" t="s">
         <v>1178</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G104" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.DeleteHorizontalWhiteSpace|N/A</v>
+      </c>
+      <c r="H104" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>376</v>
       </c>
@@ -7565,11 +7988,15 @@
       <c r="F105" t="s">
         <v>1394</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G105" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.FormatDocument|ReformatCode</v>
+      </c>
+      <c r="H105" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>376</v>
       </c>
@@ -7589,11 +8016,15 @@
       <c r="F106" t="s">
         <v>1394</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G106" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.FormatSelection|ReformatCode</v>
+      </c>
+      <c r="H106" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>376</v>
       </c>
@@ -7613,11 +8044,15 @@
       <c r="F107" t="s">
         <v>1178</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.HideSelection|N/A</v>
+      </c>
+      <c r="H107" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>376</v>
       </c>
@@ -7637,11 +8072,16 @@
       <c r="F108" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G108" s="1" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.InsertTab|EditorTab
+EditorIndentSelection</v>
+      </c>
+      <c r="H108" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>376</v>
       </c>
@@ -7661,11 +8101,15 @@
       <c r="F109" t="s">
         <v>602</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G109" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.LineCut|EditorDeleteLine</v>
+      </c>
+      <c r="H109" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>376</v>
       </c>
@@ -7685,11 +8129,15 @@
       <c r="F110" t="s">
         <v>602</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G110" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.LineDelete|EditorDeleteLine</v>
+      </c>
+      <c r="H110" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>376</v>
       </c>
@@ -7709,11 +8157,15 @@
       <c r="F111" t="s">
         <v>634</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.LineOpenAbove|EditorStartNewLineBefore</v>
+      </c>
+      <c r="H111" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>376</v>
       </c>
@@ -7733,11 +8185,15 @@
       <c r="F112" t="s">
         <v>633</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G112" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.LineOpenBelow|EditorStartNewLine</v>
+      </c>
+      <c r="H112" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>376</v>
       </c>
@@ -7754,11 +8210,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G113" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.LineTranspose|</v>
+      </c>
+      <c r="H113" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>376</v>
       </c>
@@ -7778,11 +8238,15 @@
       <c r="F114" t="s">
         <v>874</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.MakeLowercase|EditorToggleCase</v>
+      </c>
+      <c r="H114" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>376</v>
       </c>
@@ -7802,11 +8266,15 @@
       <c r="F115" t="s">
         <v>874</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G115" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.MakeUppercase|EditorToggleCase</v>
+      </c>
+      <c r="H115" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>376</v>
       </c>
@@ -7826,11 +8294,15 @@
       <c r="F116" t="s">
         <v>631</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G116" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.OvertypeMode|EditorToggleInsertState</v>
+      </c>
+      <c r="H116" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>376</v>
       </c>
@@ -7847,11 +8319,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>1</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G117" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.StopHidingCurrent|</v>
+      </c>
+      <c r="H117" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>376</v>
       </c>
@@ -7868,11 +8344,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>1</v>
       </c>
-      <c r="G118" t="s">
+      <c r="G118" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.StopOutlining|</v>
+      </c>
+      <c r="H118" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>376</v>
       </c>
@@ -7889,11 +8369,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>1</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G119" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.SwapAnchor|</v>
+      </c>
+      <c r="H119" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>376</v>
       </c>
@@ -7913,11 +8397,15 @@
       <c r="F120" t="s">
         <v>630</v>
       </c>
-      <c r="G120" t="s">
+      <c r="G120" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.TabLeft|EditorUnindentSelection</v>
+      </c>
+      <c r="H120" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>376</v>
       </c>
@@ -7937,11 +8425,16 @@
       <c r="F121" s="1" t="s">
         <v>1494</v>
       </c>
-      <c r="G121" t="s">
+      <c r="G121" s="1" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ToggleAllOutlining|CollapseAll
+ExpandAll</v>
+      </c>
+      <c r="H121" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>376</v>
       </c>
@@ -7961,11 +8454,15 @@
       <c r="F122" t="s">
         <v>628</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ToggleBookmark|ToggleBookmark</v>
+      </c>
+      <c r="H122" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>376</v>
       </c>
@@ -7982,11 +8479,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>1</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ToggleOutliningExpansion|</v>
+      </c>
+      <c r="H123" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>376</v>
       </c>
@@ -8006,11 +8507,15 @@
       <c r="F124" t="s">
         <v>1178</v>
       </c>
-      <c r="G124" t="s">
+      <c r="G124" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ToggleTaskListShortcut|N/A</v>
+      </c>
+      <c r="H124" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>376</v>
       </c>
@@ -8030,11 +8535,15 @@
       <c r="F125" t="s">
         <v>1002</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G125" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ToggleWordWrap|EditorToggleUseSoftWraps</v>
+      </c>
+      <c r="H125" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>376</v>
       </c>
@@ -8054,11 +8563,15 @@
       <c r="F126" t="s">
         <v>1219</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.UnCommentSelection|CommentByLineComment</v>
+      </c>
+      <c r="H126" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>376</v>
       </c>
@@ -8078,11 +8591,15 @@
       <c r="F127" t="s">
         <v>1001</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.ViewWhiteSpace|EditorToggleShowWhitespaces</v>
+      </c>
+      <c r="H127" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>376</v>
       </c>
@@ -8102,11 +8619,15 @@
       <c r="F128" t="s">
         <v>876</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G128" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.WordDeleteToEnd|EditorDeleteToWordEnd</v>
+      </c>
+      <c r="H128" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>376</v>
       </c>
@@ -8126,11 +8647,15 @@
       <c r="F129" t="s">
         <v>875</v>
       </c>
-      <c r="G129" t="s">
+      <c r="G129" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.WordDeleteToStart|EditorDeleteToWordStart</v>
+      </c>
+      <c r="H129" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>376</v>
       </c>
@@ -8150,11 +8675,15 @@
       <c r="F130" t="s">
         <v>1178</v>
       </c>
-      <c r="G130" t="s">
+      <c r="G130" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Manipulation Shortcut Keys|Edit.WordTranspose|N/A</v>
+      </c>
+      <c r="H130" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>441</v>
       </c>
@@ -8174,11 +8703,15 @@
       <c r="F131" t="s">
         <v>818</v>
       </c>
-      <c r="G131" t="s">
+      <c r="G131" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.CharLeft|EditorLeft</v>
+      </c>
+      <c r="H131" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>441</v>
       </c>
@@ -8198,11 +8731,15 @@
       <c r="F132" t="s">
         <v>819</v>
       </c>
-      <c r="G132" t="s">
+      <c r="G132" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.CharRight|EditorRight</v>
+      </c>
+      <c r="H132" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>441</v>
       </c>
@@ -8222,11 +8759,15 @@
       <c r="F133" t="s">
         <v>883</v>
       </c>
-      <c r="G133" t="s">
+      <c r="G133" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.DocumentEnd|EditorTextEnd</v>
+      </c>
+      <c r="H133" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>441</v>
       </c>
@@ -8246,11 +8787,15 @@
       <c r="F134" t="s">
         <v>884</v>
       </c>
-      <c r="G134" t="s">
+      <c r="G134" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.DocumentStart|EditorTextStart</v>
+      </c>
+      <c r="H134" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>441</v>
       </c>
@@ -8270,11 +8815,15 @@
       <c r="F135" t="s">
         <v>873</v>
       </c>
-      <c r="G135" t="s">
+      <c r="G135" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.GoTo|GotoLine</v>
+      </c>
+      <c r="H135" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>441</v>
       </c>
@@ -8294,11 +8843,15 @@
       <c r="F136" t="s">
         <v>1178</v>
       </c>
-      <c r="G136" t="s">
+      <c r="G136" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.GotoBrace|N/A</v>
+      </c>
+      <c r="H136" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>441</v>
       </c>
@@ -8318,11 +8871,15 @@
       <c r="F137" t="s">
         <v>877</v>
       </c>
-      <c r="G137" t="s">
+      <c r="G137" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.LineDown|EditorDown</v>
+      </c>
+      <c r="H137" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>441</v>
       </c>
@@ -8342,11 +8899,15 @@
       <c r="F138" t="s">
         <v>636</v>
       </c>
-      <c r="G138" t="s">
+      <c r="G138" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.LineEnd|EditorLineEnd</v>
+      </c>
+      <c r="H138" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>441</v>
       </c>
@@ -8366,11 +8927,15 @@
       <c r="F139" t="s">
         <v>635</v>
       </c>
-      <c r="G139" t="s">
+      <c r="G139" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.LineStart|EditorLineStart</v>
+      </c>
+      <c r="H139" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>441</v>
       </c>
@@ -8390,11 +8955,15 @@
       <c r="F140" t="s">
         <v>878</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.LineUp|EditorUp</v>
+      </c>
+      <c r="H140" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>441</v>
       </c>
@@ -8414,11 +8983,15 @@
       <c r="F141" t="s">
         <v>863</v>
       </c>
-      <c r="G141" t="s">
+      <c r="G141" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.NextBookmark|GotoNextBookmark</v>
+      </c>
+      <c r="H141" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>441</v>
       </c>
@@ -8438,11 +9011,15 @@
       <c r="F142" t="s">
         <v>821</v>
       </c>
-      <c r="G142" t="s">
+      <c r="G142" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.PageDown|EditorPageDown</v>
+      </c>
+      <c r="H142" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>441</v>
       </c>
@@ -8462,11 +9039,15 @@
       <c r="F143" t="s">
         <v>820</v>
       </c>
-      <c r="G143" t="s">
+      <c r="G143" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.PageUp|EditorPageUp</v>
+      </c>
+      <c r="H143" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>441</v>
       </c>
@@ -8486,11 +9067,15 @@
       <c r="F144" t="s">
         <v>864</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G144" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.PreviousBookmark|GotoPreviousBookmark</v>
+      </c>
+      <c r="H144" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>441</v>
       </c>
@@ -8510,11 +9095,15 @@
       <c r="F145" t="s">
         <v>1178</v>
       </c>
-      <c r="G145" t="s">
+      <c r="G145" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.QuickInfo|N/A</v>
+      </c>
+      <c r="H145" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>441</v>
       </c>
@@ -8534,11 +9123,15 @@
       <c r="F146" t="s">
         <v>902</v>
       </c>
-      <c r="G146" t="s">
+      <c r="G146" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.ScrollLineDown|EditorScrollDown</v>
+      </c>
+      <c r="H146" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>441</v>
       </c>
@@ -8558,11 +9151,15 @@
       <c r="F147" t="s">
         <v>903</v>
       </c>
-      <c r="G147" t="s">
+      <c r="G147" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.ScrollLineUp|EditorScrollUp</v>
+      </c>
+      <c r="H147" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>441</v>
       </c>
@@ -8579,11 +9176,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G148" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.ShowTileGrid|</v>
+      </c>
+      <c r="H148" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>441</v>
       </c>
@@ -8603,11 +9204,15 @@
       <c r="F149" t="s">
         <v>892</v>
       </c>
-      <c r="G149" t="s">
+      <c r="G149" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.WordNext|EditorNextWord</v>
+      </c>
+      <c r="H149" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>441</v>
       </c>
@@ -8627,11 +9232,15 @@
       <c r="F150" t="s">
         <v>891</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G150" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|Edit.WordPrevious|EditorPreviousWord</v>
+      </c>
+      <c r="H150" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>441</v>
       </c>
@@ -8649,11 +9258,15 @@
         <v>0</v>
       </c>
       <c r="F151" s="1"/>
-      <c r="G151" t="s">
+      <c r="G151" s="1" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|View.BrowseNext|</v>
+      </c>
+      <c r="H151" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>441</v>
       </c>
@@ -8671,11 +9284,15 @@
         <v>0</v>
       </c>
       <c r="F152" s="1"/>
-      <c r="G152" t="s">
+      <c r="G152" s="1" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Navigation Shortcut Keys|View.BrowsePrevious|</v>
+      </c>
+      <c r="H152" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>521</v>
       </c>
@@ -8695,11 +9312,15 @@
       <c r="F153" t="s">
         <v>880</v>
       </c>
-      <c r="G153" t="s">
+      <c r="G153" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.CharLeftExtend|EditorLeftWithSelection</v>
+      </c>
+      <c r="H153" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>521</v>
       </c>
@@ -8716,11 +9337,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G154" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.CharLeftExtendColumn|</v>
+      </c>
+      <c r="H154" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>521</v>
       </c>
@@ -8740,11 +9365,15 @@
       <c r="F155" t="s">
         <v>881</v>
       </c>
-      <c r="G155" t="s">
+      <c r="G155" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.CharRightExtend|EditorRightWithSelection</v>
+      </c>
+      <c r="H155" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>521</v>
       </c>
@@ -8761,11 +9390,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G156" t="s">
+      <c r="G156" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.CharRightExtendColumn|</v>
+      </c>
+      <c r="H156" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>521</v>
       </c>
@@ -8785,11 +9418,15 @@
       <c r="F157" t="s">
         <v>885</v>
       </c>
-      <c r="G157" t="s">
+      <c r="G157" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.DocumentEndExtend|EditorTextEndWithSelection</v>
+      </c>
+      <c r="H157" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>521</v>
       </c>
@@ -8809,11 +9446,15 @@
       <c r="F158" t="s">
         <v>886</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G158" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.DocumentStartExtend|EditorTextStartWithSelection</v>
+      </c>
+      <c r="H158" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>521</v>
       </c>
@@ -8830,11 +9471,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G159" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.GotoBraceExtend|</v>
+      </c>
+      <c r="H159" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>521</v>
       </c>
@@ -8854,11 +9499,15 @@
       <c r="F160" t="s">
         <v>882</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G160" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineDownExtend|EditorDownWithSelection</v>
+      </c>
+      <c r="H160" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>521</v>
       </c>
@@ -8878,11 +9527,15 @@
       <c r="F161" t="s">
         <v>909</v>
       </c>
-      <c r="G161" t="s">
+      <c r="G161" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineDownExtendColumn|MoveLineDown</v>
+      </c>
+      <c r="H161" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>521</v>
       </c>
@@ -8902,11 +9555,15 @@
       <c r="F162" t="s">
         <v>887</v>
       </c>
-      <c r="G162" t="s">
+      <c r="G162" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineEndExtend|EditorLineEndWithSelection</v>
+      </c>
+      <c r="H162" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>521</v>
       </c>
@@ -8923,11 +9580,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G163" t="s">
+      <c r="G163" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineEndExtendColumn|</v>
+      </c>
+      <c r="H163" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>521</v>
       </c>
@@ -8947,11 +9608,15 @@
       <c r="F164" t="s">
         <v>888</v>
       </c>
-      <c r="G164" t="s">
+      <c r="G164" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineStartExtend|EditorLineStartWithSelection</v>
+      </c>
+      <c r="H164" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>521</v>
       </c>
@@ -8968,11 +9633,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G165" t="s">
+      <c r="G165" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineStartExtendColumn|</v>
+      </c>
+      <c r="H165" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>521</v>
       </c>
@@ -8992,11 +9661,15 @@
       <c r="F166" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="G166" t="s">
+      <c r="G166" s="1" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineUpExtend|EditorUpWithSelection</v>
+      </c>
+      <c r="H166" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>521</v>
       </c>
@@ -9016,11 +9689,15 @@
       <c r="F167" t="s">
         <v>908</v>
       </c>
-      <c r="G167" t="s">
+      <c r="G167" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.LineUpExtendColumn|MoveLineUp</v>
+      </c>
+      <c r="H167" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>521</v>
       </c>
@@ -9040,11 +9717,15 @@
       <c r="F168" t="s">
         <v>897</v>
       </c>
-      <c r="G168" t="s">
+      <c r="G168" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.PageDownExtend|EditorPageDownWithSelection</v>
+      </c>
+      <c r="H168" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>521</v>
       </c>
@@ -9064,11 +9745,15 @@
       <c r="F169" t="s">
         <v>898</v>
       </c>
-      <c r="G169" t="s">
+      <c r="G169" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.PageUpExtend|EditorPageUpWithSelection</v>
+      </c>
+      <c r="H169" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>521</v>
       </c>
@@ -9088,11 +9773,15 @@
       <c r="F170" t="s">
         <v>627</v>
       </c>
-      <c r="G170" t="s">
+      <c r="G170" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.SelectAll|$SelectAll</v>
+      </c>
+      <c r="H170" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>521</v>
       </c>
@@ -9112,11 +9801,15 @@
       <c r="F171" t="s">
         <v>1179</v>
       </c>
-      <c r="G171" t="s">
+      <c r="G171" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.SelectCurrentWord|EditorSelectWord</v>
+      </c>
+      <c r="H171" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>521</v>
       </c>
@@ -9136,11 +9829,15 @@
       <c r="F172" t="s">
         <v>1178</v>
       </c>
-      <c r="G172" t="s">
+      <c r="G172" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.SelectToLastGoBack|N/A</v>
+      </c>
+      <c r="H172" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>521</v>
       </c>
@@ -9160,11 +9857,15 @@
       <c r="F173" t="s">
         <v>896</v>
       </c>
-      <c r="G173" t="s">
+      <c r="G173" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.ViewBottomExtend|EditorMoveToPageBottomWithSelection</v>
+      </c>
+      <c r="H173" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -9184,11 +9885,15 @@
       <c r="F174" t="s">
         <v>895</v>
       </c>
-      <c r="G174" t="s">
+      <c r="G174" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.ViewTopExtend|EditorMoveToPageTopWithSelection</v>
+      </c>
+      <c r="H174" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>521</v>
       </c>
@@ -9208,11 +9913,15 @@
       <c r="F175" t="s">
         <v>894</v>
       </c>
-      <c r="G175" t="s">
+      <c r="G175" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.WordNextExtend|EditorNextWordWithSelection</v>
+      </c>
+      <c r="H175" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>521</v>
       </c>
@@ -9232,11 +9941,15 @@
       <c r="F176" t="s">
         <v>911</v>
       </c>
-      <c r="G176" t="s">
+      <c r="G176" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.WordNextExtendColumn|MoveElementRight</v>
+      </c>
+      <c r="H176" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>521</v>
       </c>
@@ -9256,11 +9969,15 @@
       <c r="F177" t="s">
         <v>893</v>
       </c>
-      <c r="G177" t="s">
+      <c r="G177" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.WordPreviousExtend|EditorPreviousWordWithSelection</v>
+      </c>
+      <c r="H177" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>521</v>
       </c>
@@ -9280,11 +9997,15 @@
       <c r="F178" t="s">
         <v>910</v>
       </c>
-      <c r="G178" t="s">
+      <c r="G178" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Text Selection Shortcut Keys|Edit.WordPreviousExtendColumn|MoveElementLeft</v>
+      </c>
+      <c r="H178" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>553</v>
       </c>
@@ -9301,11 +10022,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G179" t="s">
+      <c r="G179" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|Tools.CommandWindowMarkMode|</v>
+      </c>
+      <c r="H179" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>553</v>
       </c>
@@ -9325,11 +10050,15 @@
       <c r="F180" t="s">
         <v>832</v>
       </c>
-      <c r="G180" t="s">
+      <c r="G180" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.ClassView|ActivateHierarchyToolWindow</v>
+      </c>
+      <c r="H180" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>553</v>
       </c>
@@ -9349,11 +10078,15 @@
       <c r="F181" t="s">
         <v>840</v>
       </c>
-      <c r="G181" t="s">
+      <c r="G181" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.CommandWindow|IdeScriptingConsole</v>
+      </c>
+      <c r="H181" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>553</v>
       </c>
@@ -9373,11 +10106,15 @@
       <c r="F182" t="s">
         <v>827</v>
       </c>
-      <c r="G182" t="s">
+      <c r="G182" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.DocumentOutline|ActivateStructureToolWindow</v>
+      </c>
+      <c r="H182" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>553</v>
       </c>
@@ -9397,11 +10134,15 @@
       <c r="F183" t="s">
         <v>826</v>
       </c>
-      <c r="G183" t="s">
+      <c r="G183" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.Favorites|ActivateFavoritesToolWindow</v>
+      </c>
+      <c r="H183" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>553</v>
       </c>
@@ -9421,11 +10162,15 @@
       <c r="F184" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="G184" t="s">
+      <c r="G184" s="1" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.Output|ActivateRunToolWindow</v>
+      </c>
+      <c r="H184" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>553</v>
       </c>
@@ -9445,11 +10190,15 @@
       <c r="F185" t="s">
         <v>1178</v>
       </c>
-      <c r="G185" t="s">
+      <c r="G185" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.PropertiesWindow|N/A</v>
+      </c>
+      <c r="H185" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>553</v>
       </c>
@@ -9466,11 +10215,15 @@
         <f>ISNUMBER(FIND(",",Table1[[#This Row],[VC_Shortcut_Keys]]))</f>
         <v>0</v>
       </c>
-      <c r="G186" t="s">
+      <c r="G186" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.ResourceView|</v>
+      </c>
+      <c r="H186" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>553</v>
       </c>
@@ -9490,11 +10243,15 @@
       <c r="F187" t="s">
         <v>842</v>
       </c>
-      <c r="G187" t="s">
+      <c r="G187" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.ServerExplorer|ActivateDatabaseToolWindow</v>
+      </c>
+      <c r="H187" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>553</v>
       </c>
@@ -9514,11 +10271,15 @@
       <c r="F188" t="s">
         <v>833</v>
       </c>
-      <c r="G188" t="s">
+      <c r="G188" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.SolutionExplorer|ActivateProjectToolWindow</v>
+      </c>
+      <c r="H188" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>553</v>
       </c>
@@ -9538,11 +10299,15 @@
       <c r="F189" t="s">
         <v>841</v>
       </c>
-      <c r="G189" t="s">
+      <c r="G189" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.TaskList|ActivateTODOToolWindow</v>
+      </c>
+      <c r="H189" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>553</v>
       </c>
@@ -9562,11 +10327,15 @@
       <c r="F190" t="s">
         <v>1178</v>
       </c>
-      <c r="G190" t="s">
+      <c r="G190" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Tool Window Shortcut Keys|View.Toolbox|N/A</v>
+      </c>
+      <c r="H190" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>595</v>
       </c>
@@ -9586,11 +10355,15 @@
       <c r="F191" t="s">
         <v>843</v>
       </c>
-      <c r="G191" t="s">
+      <c r="G191" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|View.FullScreen|ToggleFullScreen</v>
+      </c>
+      <c r="H191" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>595</v>
       </c>
@@ -9610,11 +10383,15 @@
       <c r="F192" t="s">
         <v>830</v>
       </c>
-      <c r="G192" t="s">
+      <c r="G192" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|View.NavigateBackward|Back</v>
+      </c>
+      <c r="H192" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>595</v>
       </c>
@@ -9634,11 +10411,15 @@
       <c r="F193" t="s">
         <v>831</v>
       </c>
-      <c r="G193" t="s">
+      <c r="G193" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|View.NavigateForward|Forward</v>
+      </c>
+      <c r="H193" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>595</v>
       </c>
@@ -9658,11 +10439,15 @@
       <c r="F194" t="s">
         <v>834</v>
       </c>
-      <c r="G194" t="s">
+      <c r="G194" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.ActivateDocumentWindow|FocusEditor</v>
+      </c>
+      <c r="H194" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>595</v>
       </c>
@@ -9682,11 +10467,15 @@
       <c r="F195" t="s">
         <v>845</v>
       </c>
-      <c r="G195" t="s">
+      <c r="G195" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.CloseDocumentWindow|CloseContent</v>
+      </c>
+      <c r="H195" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>595</v>
       </c>
@@ -9706,11 +10495,15 @@
       <c r="F196" t="s">
         <v>844</v>
       </c>
-      <c r="G196" t="s">
+      <c r="G196" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.CloseToolWindow|HideActiveWindow</v>
+      </c>
+      <c r="H196" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>595</v>
       </c>
@@ -9730,11 +10523,15 @@
       <c r="F197" t="s">
         <v>848</v>
       </c>
-      <c r="G197" t="s">
+      <c r="G197" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.NextDocumentWindow|NextTab</v>
+      </c>
+      <c r="H197" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>595</v>
       </c>
@@ -9754,11 +10551,15 @@
       <c r="F198" t="s">
         <v>846</v>
       </c>
-      <c r="G198" t="s">
+      <c r="G198" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.NextPane|NextSplitter</v>
+      </c>
+      <c r="H198" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>595</v>
       </c>
@@ -9778,11 +10579,15 @@
       <c r="F199" t="s">
         <v>846</v>
       </c>
-      <c r="G199" t="s">
+      <c r="G199" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.NextSplitPane|NextSplitter</v>
+      </c>
+      <c r="H199" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>595</v>
       </c>
@@ -9802,11 +10607,15 @@
       <c r="F200" t="s">
         <v>848</v>
       </c>
-      <c r="G200" t="s">
+      <c r="G200" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.NextTab|NextTab</v>
+      </c>
+      <c r="H200" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>595</v>
       </c>
@@ -9826,11 +10635,15 @@
       <c r="F201" t="s">
         <v>849</v>
       </c>
-      <c r="G201" t="s">
+      <c r="G201" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.PreviousDocumentWindow|PreviousTab</v>
+      </c>
+      <c r="H201" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>595</v>
       </c>
@@ -9850,11 +10663,15 @@
       <c r="F202" t="s">
         <v>847</v>
       </c>
-      <c r="G202" t="s">
+      <c r="G202" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.PreviousPane|PrevSplitter</v>
+      </c>
+      <c r="H202" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>595</v>
       </c>
@@ -9874,11 +10691,15 @@
       <c r="F203" t="s">
         <v>847</v>
       </c>
-      <c r="G203" t="s">
+      <c r="G203" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.PreviousSplitPane|PrevSplitter</v>
+      </c>
+      <c r="H203" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>595</v>
       </c>
@@ -9898,7 +10719,11 @@
       <c r="F204" t="s">
         <v>849</v>
       </c>
-      <c r="G204" t="s">
+      <c r="G204" t="str">
+        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
+        <v>Window Management Shortcut Keys|Window.PreviousTab|PreviousTab</v>
+      </c>
+      <c r="H204" t="s">
         <v>594</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix broken table MD in readme.
</commit_message>
<xml_diff>
--- a/WellEngineered.us VC++ 6.0 Shortcuts.xlsx
+++ b/WellEngineered.us VC++ 6.0 Shortcuts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B3E717-587A-4343-98E7-A2B47D99A69F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D53B95E-78D2-4CD9-A8D8-DF3BC048471E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5D8658FC-F053-4B4D-BC9B-4C701ADA3E99}"/>
   </bookViews>
@@ -4789,7 +4789,7 @@
     </tableColumn>
     <tableColumn id="7" xr3:uid="{AD3AB443-69FC-4ED6-9DE9-F3E9E01AD994}" name="IDEA_Keymap_ID"/>
     <tableColumn id="8" xr3:uid="{9C6E70BC-6004-42BB-8E99-008FFF3A215B}" name="Column1" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</calculatedColumnFormula>
+      <calculatedColumnFormula>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{4EBEDB49-82CC-456A-8155-4D2F3CD27D4E}" name="Description"/>
   </tableColumns>
@@ -5096,7 +5096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D07097-255A-46B5-AC8C-91A030E6460F}">
   <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5157,8 +5159,8 @@
         <v>1178</v>
       </c>
       <c r="G2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.ApplyCodeChanges|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ApplyCodeChanges|N/A|</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>67</v>
@@ -5185,8 +5187,8 @@
         <v>1178</v>
       </c>
       <c r="G3" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Autos|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Autos|N/A|</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>70</v>
@@ -5213,8 +5215,8 @@
         <v>871</v>
       </c>
       <c r="G4" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.BreakAll|Pause</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.BreakAll|Pause|</v>
       </c>
       <c r="H4" t="s">
         <v>73</v>
@@ -5241,8 +5243,8 @@
         <v>837</v>
       </c>
       <c r="G5" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Breakpoints|ViewBreakpoints</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Breakpoints|ViewBreakpoints|</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>76</v>
@@ -5269,8 +5271,8 @@
         <v>1178</v>
       </c>
       <c r="G6" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.CallStack|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.CallStack|N/A|</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>79</v>
@@ -5297,8 +5299,8 @@
         <v>1040</v>
       </c>
       <c r="G7" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.ClearAllBreakpoints|RiderRemoveAllLineBreakpoints</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ClearAllBreakpoints|RiderRemoveAllLineBreakpoints|</v>
       </c>
       <c r="H7" t="s">
         <v>82</v>
@@ -5325,8 +5327,8 @@
         <v>851</v>
       </c>
       <c r="G8" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Continue ***|Resume</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Continue ***|Resume|</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -5351,8 +5353,8 @@
         <v>858</v>
       </c>
       <c r="G9" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Disassembly|ActivateILViewerToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Disassembly|ActivateILViewerToolWindow|</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>85</v>
@@ -5379,8 +5381,8 @@
         <v>853</v>
       </c>
       <c r="G10" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.EnableBreakpoint|ToggleBreakpointEnabled</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.EnableBreakpoint|ToggleBreakpointEnabled|</v>
       </c>
       <c r="H10" t="s">
         <v>88</v>
@@ -5407,8 +5409,8 @@
         <v>1490</v>
       </c>
       <c r="G11" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Exceptions|OpenExceptionSettings</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Exceptions|OpenExceptionSettings|</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>91</v>
@@ -5435,8 +5437,8 @@
         <v>1491</v>
       </c>
       <c r="G12" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Immediate|NavigateToImmediateWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Immediate|NavigateToImmediateWindow|</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>610</v>
@@ -5463,8 +5465,8 @@
         <v>1178</v>
       </c>
       <c r="G13" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Locals|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Locals|N/A|</v>
       </c>
       <c r="H13" t="s">
         <v>95</v>
@@ -5491,8 +5493,8 @@
         <v>1178</v>
       </c>
       <c r="G14" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Memory1|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory1|N/A|</v>
       </c>
       <c r="H14" t="s">
         <v>98</v>
@@ -5519,8 +5521,8 @@
         <v>1178</v>
       </c>
       <c r="G15" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Memory2|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory2|N/A|</v>
       </c>
       <c r="H15" t="s">
         <v>101</v>
@@ -5547,8 +5549,8 @@
         <v>1178</v>
       </c>
       <c r="G16" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Memory3|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory3|N/A|</v>
       </c>
       <c r="H16" t="s">
         <v>104</v>
@@ -5575,8 +5577,8 @@
         <v>1178</v>
       </c>
       <c r="G17" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Memory4|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory4|N/A|</v>
       </c>
       <c r="H17" t="s">
         <v>107</v>
@@ -5603,8 +5605,8 @@
         <v>1178</v>
       </c>
       <c r="G18" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Modules|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Modules|N/A|</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>110</v>
@@ -5631,8 +5633,8 @@
         <v>855</v>
       </c>
       <c r="G19" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.NewBreakpoint|ToggleTemporaryLineBreakpoint</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.NewBreakpoint|ToggleTemporaryLineBreakpoint|</v>
       </c>
       <c r="H19" t="s">
         <v>113</v>
@@ -5659,8 +5661,8 @@
         <v>1178</v>
       </c>
       <c r="G20" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.QuickWatch|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.QuickWatch|N/A|</v>
       </c>
       <c r="H20" t="s">
         <v>611</v>
@@ -5687,8 +5689,8 @@
         <v>1178</v>
       </c>
       <c r="G21" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Registers|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Registers|N/A|</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>118</v>
@@ -5715,8 +5717,8 @@
         <v>1178</v>
       </c>
       <c r="G22" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Restart|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Restart|N/A|</v>
       </c>
       <c r="H22" t="s">
         <v>121</v>
@@ -5743,8 +5745,8 @@
         <v>1178</v>
       </c>
       <c r="G23" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.RunningDocuments|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.RunningDocuments|N/A|</v>
       </c>
       <c r="H23" t="s">
         <v>124</v>
@@ -5771,8 +5773,8 @@
         <v>857</v>
       </c>
       <c r="G24" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.RunToCursor|RunToCursor</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.RunToCursor|RunToCursor|</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>127</v>
@@ -5799,8 +5801,8 @@
         <v>1178</v>
       </c>
       <c r="G25" s="2" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.SetNextStatement|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.SetNextStatement|N/A|</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>130</v>
@@ -5827,8 +5829,8 @@
         <v>854</v>
       </c>
       <c r="G26" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.ShowNextStatement|ShowExecutionPoint</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ShowNextStatement|ShowExecutionPoint|</v>
       </c>
       <c r="H26" t="s">
         <v>133</v>
@@ -5855,8 +5857,8 @@
         <v>872</v>
       </c>
       <c r="G27" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Start (Continue)|#</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Start (Continue)|#|</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>135</v>
@@ -5883,8 +5885,8 @@
         <v>850</v>
       </c>
       <c r="G28" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Start ***|Debug</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Start ***|Debug|</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -5909,8 +5911,8 @@
         <v>856</v>
       </c>
       <c r="G29" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.StartWithoutDebugging|Run</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StartWithoutDebugging|Run|</v>
       </c>
       <c r="H29" t="s">
         <v>138</v>
@@ -5937,8 +5939,8 @@
         <v>859</v>
       </c>
       <c r="G30" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.StepInto|StepInto</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StepInto|StepInto|</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>141</v>
@@ -5965,8 +5967,8 @@
         <v>860</v>
       </c>
       <c r="G31" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.StepOut|StepOut</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StepOut|StepOut|</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>144</v>
@@ -5993,8 +5995,8 @@
         <v>861</v>
       </c>
       <c r="G32" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.StepOver|StepOver</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StepOver|StepOver|</v>
       </c>
       <c r="H32" t="s">
         <v>147</v>
@@ -6021,8 +6023,8 @@
         <v>862</v>
       </c>
       <c r="G33" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.StopDebugging|Stop</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StopDebugging|Stop|</v>
       </c>
       <c r="H33" t="s">
         <v>150</v>
@@ -6049,8 +6051,8 @@
         <v>1178</v>
       </c>
       <c r="G34" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.This|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.This|N/A|</v>
       </c>
       <c r="H34" t="s">
         <v>153</v>
@@ -6077,8 +6079,8 @@
         <v>1178</v>
       </c>
       <c r="G35" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.Threads|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Threads|N/A|</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>156</v>
@@ -6105,8 +6107,8 @@
         <v>852</v>
       </c>
       <c r="G36" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.ToggleBreakpoint|ToggleLineBreakpoint</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ToggleBreakpoint|ToggleLineBreakpoint|</v>
       </c>
       <c r="H36" t="s">
         <v>159</v>
@@ -6133,8 +6135,8 @@
         <v>1178</v>
       </c>
       <c r="G37" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Debug.ToggleDisassembly|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ToggleDisassembly|N/A|</v>
       </c>
       <c r="H37" t="s">
         <v>162</v>
@@ -6161,8 +6163,8 @@
         <v>836</v>
       </c>
       <c r="G38" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Debug Shortcut Keys|Tools.DebugProcesses|XDebugger.AttachToProcess</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Debug Shortcut Keys|Tools.DebugProcesses|XDebugger.AttachToProcess|</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>165</v>
@@ -6189,8 +6191,8 @@
         <v>622</v>
       </c>
       <c r="G39" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.Copy|$Copy</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Copy|$Copy|</v>
       </c>
       <c r="H39" t="s">
         <v>4</v>
@@ -6217,8 +6219,8 @@
         <v>623</v>
       </c>
       <c r="G40" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.Cut|$Cut</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Cut|$Cut|</v>
       </c>
       <c r="H40" t="s">
         <v>7</v>
@@ -6245,8 +6247,8 @@
         <v>1178</v>
       </c>
       <c r="G41" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.CycleClipboardRing|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.CycleClipboardRing|N/A|</v>
       </c>
       <c r="H41" t="s">
         <v>7</v>
@@ -6273,8 +6275,8 @@
         <v>1181</v>
       </c>
       <c r="G42" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.GotoNextLocation|GotoNextError</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.GotoNextLocation|GotoNextError|</v>
       </c>
       <c r="H42" t="s">
         <v>63</v>
@@ -6301,8 +6303,8 @@
         <v>1182</v>
       </c>
       <c r="G43" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.GotoPreviousLocation|GotoPreviousError</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.GotoPreviousLocation|GotoPreviousError|</v>
       </c>
       <c r="H43" t="s">
         <v>17</v>
@@ -6326,8 +6328,8 @@
         <v>0</v>
       </c>
       <c r="G44" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.GoToReference|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.GoToReference||</v>
       </c>
       <c r="H44" t="s">
         <v>20</v>
@@ -6351,8 +6353,8 @@
         <v>0</v>
       </c>
       <c r="G45" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.ListMembers|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.ListMembers||</v>
       </c>
       <c r="H45" t="s">
         <v>12</v>
@@ -6379,8 +6381,8 @@
         <v>624</v>
       </c>
       <c r="G46" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.Paste|$Paste</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Paste|$Paste|</v>
       </c>
       <c r="H46" t="s">
         <v>23</v>
@@ -6407,8 +6409,8 @@
         <v>625</v>
       </c>
       <c r="G47" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.Redo|$Redo</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Redo|$Redo|</v>
       </c>
       <c r="H47" t="s">
         <v>26</v>
@@ -6435,8 +6437,8 @@
         <v>637</v>
       </c>
       <c r="G48" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.SelectionCancel|EditorEscape</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.SelectionCancel|EditorEscape|</v>
       </c>
       <c r="H48" t="s">
         <v>29</v>
@@ -6463,8 +6465,8 @@
         <v>626</v>
       </c>
       <c r="G49" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Edit.Undo|$Undo</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Undo|$Undo|</v>
       </c>
       <c r="H49" t="s">
         <v>32</v>
@@ -6491,8 +6493,8 @@
         <v>838</v>
       </c>
       <c r="G50" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|File.Print|Print</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|File.Print|Print|</v>
       </c>
       <c r="H50" t="s">
         <v>35</v>
@@ -6519,8 +6521,8 @@
         <v>835</v>
       </c>
       <c r="G51" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|File.SaveAll|SaveAll</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|File.SaveAll|SaveAll|</v>
       </c>
       <c r="H51" t="s">
         <v>38</v>
@@ -6547,8 +6549,8 @@
         <v>839</v>
       </c>
       <c r="G52" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|File.SaveSelectedItems|SaveDocument</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|File.SaveSelectedItems|SaveDocument|</v>
       </c>
       <c r="H52" t="s">
         <v>41</v>
@@ -6575,8 +6577,8 @@
         <v>1178</v>
       </c>
       <c r="G53" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|Tools.GoToCommandLine|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|Tools.GoToCommandLine|N/A|</v>
       </c>
       <c r="H53" t="s">
         <v>613</v>
@@ -6600,8 +6602,8 @@
         <v>0</v>
       </c>
       <c r="G54" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.NextTask|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.NextTask||</v>
       </c>
       <c r="H54" t="s">
         <v>45</v>
@@ -6625,8 +6627,8 @@
         <v>0</v>
       </c>
       <c r="G55" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.PopBrowseContext|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.PopBrowseContext||</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>64</v>
@@ -6650,8 +6652,8 @@
         <v>0</v>
       </c>
       <c r="G56" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.PreviousTask|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.PreviousTask||</v>
       </c>
       <c r="H56" t="s">
         <v>50</v>
@@ -6678,8 +6680,8 @@
         <v>1178</v>
       </c>
       <c r="G57" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.ViewCode|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.ViewCode|N/A|</v>
       </c>
       <c r="H57" t="s">
         <v>53</v>
@@ -6706,8 +6708,8 @@
         <v>1178</v>
       </c>
       <c r="G58" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.ViewDesigner|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.ViewDesigner|N/A|</v>
       </c>
       <c r="H58" t="s">
         <v>56</v>
@@ -6734,8 +6736,8 @@
         <v>830</v>
       </c>
       <c r="G59" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.WebNavigateBack|Back</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.WebNavigateBack|Back|</v>
       </c>
       <c r="H59" t="s">
         <v>59</v>
@@ -6762,8 +6764,8 @@
         <v>831</v>
       </c>
       <c r="G60" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Global Shortcut Keys|View.WebNavigateForward|Forward</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Global Shortcut Keys|View.WebNavigateForward|Forward|</v>
       </c>
       <c r="H60" t="s">
         <v>62</v>
@@ -6790,8 +6792,8 @@
         <v>1338</v>
       </c>
       <c r="G61" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|Edit.FindSymbol|GotoSymbol</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|Edit.FindSymbol|GotoSymbol|</v>
       </c>
       <c r="H61" t="s">
         <v>271</v>
@@ -6815,8 +6817,8 @@
         <v>0</v>
       </c>
       <c r="G62" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|Edit.GoToDeclaration|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|Edit.GoToDeclaration||</v>
       </c>
       <c r="H62" t="s">
         <v>256</v>
@@ -6843,8 +6845,8 @@
         <v>1180</v>
       </c>
       <c r="G63" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|Edit.GoToDefinition|GotoDeclaration</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|Edit.GoToDefinition|GotoDeclaration|</v>
       </c>
       <c r="H63" t="s">
         <v>259</v>
@@ -6868,8 +6870,8 @@
         <v>0</v>
       </c>
       <c r="G64" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|View.FindSymbolResults|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.FindSymbolResults||</v>
       </c>
       <c r="H64" t="s">
         <v>272</v>
@@ -6896,8 +6898,8 @@
         <v>1178</v>
       </c>
       <c r="G65" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|View.ObjectBrowser|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.ObjectBrowser|N/A|</v>
       </c>
       <c r="H65" t="s">
         <v>264</v>
@@ -6924,8 +6926,8 @@
         <v>1178</v>
       </c>
       <c r="G66" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|View.ObjectBrowserBack|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.ObjectBrowserBack|N/A|</v>
       </c>
       <c r="H66" t="s">
         <v>267</v>
@@ -6949,8 +6951,8 @@
         <v>0</v>
       </c>
       <c r="G67" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Object Browser Shortcut Keys|View.ObjectBrowserForward|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.ObjectBrowserForward||</v>
       </c>
       <c r="H67" t="s">
         <v>270</v>
@@ -6977,8 +6979,8 @@
         <v>865</v>
       </c>
       <c r="G68" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|Build.BuildSolution|BuildSolutionAction</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|Build.BuildSolution|BuildSolutionAction|</v>
       </c>
       <c r="H68" t="s">
         <v>168</v>
@@ -7005,8 +7007,8 @@
         <v>866</v>
       </c>
       <c r="G69" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|Build.Cancel|CancelBuildAction</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|Build.Cancel|CancelBuildAction|</v>
       </c>
       <c r="H69" t="s">
         <v>171</v>
@@ -7033,8 +7035,8 @@
         <v>867</v>
       </c>
       <c r="G70" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|Build.Compile|RebuildSolutionAction</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|Build.Compile|RebuildSolutionAction|</v>
       </c>
       <c r="H70" t="s">
         <v>174</v>
@@ -7058,8 +7060,8 @@
         <v>0</v>
       </c>
       <c r="G71" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|File.AddExistingItem|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|File.AddExistingItem||</v>
       </c>
       <c r="H71" t="s">
         <v>189</v>
@@ -7083,8 +7085,8 @@
         <v>0</v>
       </c>
       <c r="G72" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|File.AddNewItem|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|File.AddNewItem||</v>
       </c>
       <c r="H72" t="s">
         <v>192</v>
@@ -7111,8 +7113,8 @@
         <v>869</v>
       </c>
       <c r="G73" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|File.NewFile|NewElement</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|File.NewFile|NewElement|</v>
       </c>
       <c r="H73" t="s">
         <v>177</v>
@@ -7139,8 +7141,8 @@
         <v>989</v>
       </c>
       <c r="G74" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|File.NewProject|NewProject</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|File.NewProject|NewProject|</v>
       </c>
       <c r="H74" t="s">
         <v>180</v>
@@ -7167,8 +7169,8 @@
         <v>870</v>
       </c>
       <c r="G75" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|File.OpenFile|OpenFile</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|File.OpenFile|OpenFile|</v>
       </c>
       <c r="H75" t="s">
         <v>183</v>
@@ -7195,8 +7197,8 @@
         <v>1039</v>
       </c>
       <c r="G76" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|File.OpenProject|RiderOpenSolution</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|File.OpenProject|RiderOpenSolution|</v>
       </c>
       <c r="H76" t="s">
         <v>186</v>
@@ -7223,8 +7225,8 @@
         <v>868</v>
       </c>
       <c r="G77" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Project Shortcut Keys|Project.Override|OverrideMethods</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Project Shortcut Keys|Project.Override|OverrideMethods|</v>
       </c>
       <c r="H77" t="s">
         <v>195</v>
@@ -7251,8 +7253,8 @@
         <v>904</v>
       </c>
       <c r="G78" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.Find|Find</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Find|Find|</v>
       </c>
       <c r="H78" t="s">
         <v>198</v>
@@ -7279,8 +7281,8 @@
         <v>905</v>
       </c>
       <c r="G79" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.FindinFiles|FindInPath</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindinFiles|FindInPath|</v>
       </c>
       <c r="H79" t="s">
         <v>201</v>
@@ -7307,8 +7309,8 @@
         <v>906</v>
       </c>
       <c r="G80" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.FindNext|FindNext</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindNext|FindNext|</v>
       </c>
       <c r="H80" t="s">
         <v>204</v>
@@ -7332,8 +7334,8 @@
         <v>0</v>
       </c>
       <c r="G81" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.FindNextSelected|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindNextSelected||</v>
       </c>
       <c r="H81" t="s">
         <v>207</v>
@@ -7360,8 +7362,8 @@
         <v>907</v>
       </c>
       <c r="G82" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.FindPrevious|FindPrevious</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindPrevious|FindPrevious|</v>
       </c>
       <c r="H82" t="s">
         <v>210</v>
@@ -7385,8 +7387,8 @@
         <v>0</v>
       </c>
       <c r="G83" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.FindPreviousSelected|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindPreviousSelected||</v>
       </c>
       <c r="H83" t="s">
         <v>213</v>
@@ -7413,8 +7415,8 @@
         <v>1178</v>
       </c>
       <c r="G84" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.GoToFindCombo|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.GoToFindCombo|N/A|</v>
       </c>
       <c r="H84" t="s">
         <v>614</v>
@@ -7441,8 +7443,8 @@
         <v>1178</v>
       </c>
       <c r="G85" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.HiddenText|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.HiddenText|N/A|</v>
       </c>
       <c r="H85" t="s">
         <v>218</v>
@@ -7466,8 +7468,8 @@
         <v>0</v>
       </c>
       <c r="G86" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.IncrementalSearch|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.IncrementalSearch||</v>
       </c>
       <c r="H86" t="s">
         <v>221</v>
@@ -7494,8 +7496,8 @@
         <v>1178</v>
       </c>
       <c r="G87" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.MatchCase|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.MatchCase|N/A|</v>
       </c>
       <c r="H87" t="s">
         <v>224</v>
@@ -7522,8 +7524,8 @@
         <v>1178</v>
       </c>
       <c r="G88" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.RegularExpression|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.RegularExpression|N/A|</v>
       </c>
       <c r="H88" t="s">
         <v>227</v>
@@ -7550,8 +7552,8 @@
         <v>912</v>
       </c>
       <c r="G89" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.Replace|Replace</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Replace|Replace|</v>
       </c>
       <c r="H89" t="s">
         <v>230</v>
@@ -7578,8 +7580,8 @@
         <v>913</v>
       </c>
       <c r="G90" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.ReplaceinFiles|ReplaceInPath</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.ReplaceinFiles|ReplaceInPath|</v>
       </c>
       <c r="H90" t="s">
         <v>233</v>
@@ -7603,8 +7605,8 @@
         <v>0</v>
       </c>
       <c r="G91" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.ReverseIncrementalSearch|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.ReverseIncrementalSearch||</v>
       </c>
       <c r="H91" t="s">
         <v>236</v>
@@ -7631,8 +7633,8 @@
         <v>1178</v>
       </c>
       <c r="G92" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.StopSearch|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.StopSearch|N/A|</v>
       </c>
       <c r="H92" t="s">
         <v>239</v>
@@ -7659,8 +7661,8 @@
         <v>1178</v>
       </c>
       <c r="G93" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.Up|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Up|N/A|</v>
       </c>
       <c r="H93" t="s">
         <v>242</v>
@@ -7687,8 +7689,8 @@
         <v>1178</v>
       </c>
       <c r="G94" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.WholeWord|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.WholeWord|N/A|</v>
       </c>
       <c r="H94" t="s">
         <v>245</v>
@@ -7715,8 +7717,8 @@
         <v>1178</v>
       </c>
       <c r="G95" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Search and Replace Shortcut Keys|Edit.Wildcard|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Wildcard|N/A|</v>
       </c>
       <c r="H95" t="s">
         <v>274</v>
@@ -7743,8 +7745,8 @@
         <v>629</v>
       </c>
       <c r="G96" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.BreakLine|EditorEnter</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.BreakLine|EditorEnter|</v>
       </c>
       <c r="H96" t="s">
         <v>277</v>
@@ -7771,8 +7773,8 @@
         <v>974</v>
       </c>
       <c r="G97" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.CharTranspose|EditorTranspose</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CharTranspose|EditorTranspose|</v>
       </c>
       <c r="H97" t="s">
         <v>280</v>
@@ -7796,8 +7798,8 @@
         <v>1</v>
       </c>
       <c r="G98" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ClearBookmarks|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ClearBookmarks||</v>
       </c>
       <c r="H98" t="s">
         <v>283</v>
@@ -7821,8 +7823,8 @@
         <v>1</v>
       </c>
       <c r="G99" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.CollapsetoDefinitions|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CollapsetoDefinitions||</v>
       </c>
       <c r="H99" t="s">
         <v>286</v>
@@ -7849,8 +7851,8 @@
         <v>1219</v>
       </c>
       <c r="G100" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.CommentSelection|CommentByLineComment</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CommentSelection|CommentByLineComment|</v>
       </c>
       <c r="H100" t="s">
         <v>1493</v>
@@ -7877,8 +7879,8 @@
         <v>879</v>
       </c>
       <c r="G101" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.CompleteWord|CodeCompletion</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CompleteWord|CodeCompletion|</v>
       </c>
       <c r="H101" t="s">
         <v>290</v>
@@ -7905,8 +7907,8 @@
         <v>603</v>
       </c>
       <c r="G102" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.Delete|$Delete</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.Delete|$Delete|</v>
       </c>
       <c r="H102" t="s">
         <v>293</v>
@@ -7933,8 +7935,8 @@
         <v>632</v>
       </c>
       <c r="G103" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.DeleteBackwards|EditorBackSpace</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.DeleteBackwards|EditorBackSpace|</v>
       </c>
       <c r="H103" t="s">
         <v>296</v>
@@ -7961,8 +7963,8 @@
         <v>1178</v>
       </c>
       <c r="G104" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.DeleteHorizontalWhiteSpace|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.DeleteHorizontalWhiteSpace|N/A|</v>
       </c>
       <c r="H104" t="s">
         <v>299</v>
@@ -7989,8 +7991,8 @@
         <v>1394</v>
       </c>
       <c r="G105" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.FormatDocument|ReformatCode</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.FormatDocument|ReformatCode|</v>
       </c>
       <c r="H105" t="s">
         <v>302</v>
@@ -8017,8 +8019,8 @@
         <v>1394</v>
       </c>
       <c r="G106" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.FormatSelection|ReformatCode</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.FormatSelection|ReformatCode|</v>
       </c>
       <c r="H106" t="s">
         <v>305</v>
@@ -8045,14 +8047,14 @@
         <v>1178</v>
       </c>
       <c r="G107" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.HideSelection|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.HideSelection|N/A|</v>
       </c>
       <c r="H107" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>376</v>
       </c>
@@ -8073,9 +8075,9 @@
         <v>822</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.InsertTab|EditorTab
-EditorIndentSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.InsertTab|EditorTab
+EditorIndentSelection|</v>
       </c>
       <c r="H108" t="s">
         <v>311</v>
@@ -8102,8 +8104,8 @@
         <v>602</v>
       </c>
       <c r="G109" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.LineCut|EditorDeleteLine</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineCut|EditorDeleteLine|</v>
       </c>
       <c r="H109" t="s">
         <v>314</v>
@@ -8130,8 +8132,8 @@
         <v>602</v>
       </c>
       <c r="G110" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.LineDelete|EditorDeleteLine</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineDelete|EditorDeleteLine|</v>
       </c>
       <c r="H110" t="s">
         <v>317</v>
@@ -8158,8 +8160,8 @@
         <v>634</v>
       </c>
       <c r="G111" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.LineOpenAbove|EditorStartNewLineBefore</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineOpenAbove|EditorStartNewLineBefore|</v>
       </c>
       <c r="H111" t="s">
         <v>320</v>
@@ -8186,8 +8188,8 @@
         <v>633</v>
       </c>
       <c r="G112" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.LineOpenBelow|EditorStartNewLine</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineOpenBelow|EditorStartNewLine|</v>
       </c>
       <c r="H112" t="s">
         <v>323</v>
@@ -8211,8 +8213,8 @@
         <v>0</v>
       </c>
       <c r="G113" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.LineTranspose|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineTranspose||</v>
       </c>
       <c r="H113" t="s">
         <v>326</v>
@@ -8239,8 +8241,8 @@
         <v>874</v>
       </c>
       <c r="G114" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.MakeLowercase|EditorToggleCase</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.MakeLowercase|EditorToggleCase|</v>
       </c>
       <c r="H114" t="s">
         <v>329</v>
@@ -8267,8 +8269,8 @@
         <v>874</v>
       </c>
       <c r="G115" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.MakeUppercase|EditorToggleCase</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.MakeUppercase|EditorToggleCase|</v>
       </c>
       <c r="H115" t="s">
         <v>332</v>
@@ -8295,8 +8297,8 @@
         <v>631</v>
       </c>
       <c r="G116" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.OvertypeMode|EditorToggleInsertState</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.OvertypeMode|EditorToggleInsertState|</v>
       </c>
       <c r="H116" t="s">
         <v>335</v>
@@ -8320,8 +8322,8 @@
         <v>1</v>
       </c>
       <c r="G117" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.StopHidingCurrent|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.StopHidingCurrent||</v>
       </c>
       <c r="H117" t="s">
         <v>338</v>
@@ -8345,8 +8347,8 @@
         <v>1</v>
       </c>
       <c r="G118" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.StopOutlining|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.StopOutlining||</v>
       </c>
       <c r="H118" t="s">
         <v>341</v>
@@ -8370,8 +8372,8 @@
         <v>1</v>
       </c>
       <c r="G119" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.SwapAnchor|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.SwapAnchor||</v>
       </c>
       <c r="H119" t="s">
         <v>344</v>
@@ -8398,14 +8400,14 @@
         <v>630</v>
       </c>
       <c r="G120" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.TabLeft|EditorUnindentSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.TabLeft|EditorUnindentSelection|</v>
       </c>
       <c r="H120" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>376</v>
       </c>
@@ -8426,9 +8428,9 @@
         <v>1494</v>
       </c>
       <c r="G121" s="1" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ToggleAllOutlining|CollapseAll
-ExpandAll</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleAllOutlining|CollapseAll
+ExpandAll|</v>
       </c>
       <c r="H121" t="s">
         <v>350</v>
@@ -8455,8 +8457,8 @@
         <v>628</v>
       </c>
       <c r="G122" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ToggleBookmark|ToggleBookmark</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleBookmark|ToggleBookmark|</v>
       </c>
       <c r="H122" t="s">
         <v>353</v>
@@ -8480,8 +8482,8 @@
         <v>1</v>
       </c>
       <c r="G123" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ToggleOutliningExpansion|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleOutliningExpansion||</v>
       </c>
       <c r="H123" t="s">
         <v>356</v>
@@ -8508,8 +8510,8 @@
         <v>1178</v>
       </c>
       <c r="G124" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ToggleTaskListShortcut|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleTaskListShortcut|N/A|</v>
       </c>
       <c r="H124" t="s">
         <v>359</v>
@@ -8536,8 +8538,8 @@
         <v>1002</v>
       </c>
       <c r="G125" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ToggleWordWrap|EditorToggleUseSoftWraps</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleWordWrap|EditorToggleUseSoftWraps|</v>
       </c>
       <c r="H125" t="s">
         <v>362</v>
@@ -8564,8 +8566,8 @@
         <v>1219</v>
       </c>
       <c r="G126" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.UnCommentSelection|CommentByLineComment</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.UnCommentSelection|CommentByLineComment|</v>
       </c>
       <c r="H126" t="s">
         <v>617</v>
@@ -8592,8 +8594,8 @@
         <v>1001</v>
       </c>
       <c r="G127" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.ViewWhiteSpace|EditorToggleShowWhitespaces</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ViewWhiteSpace|EditorToggleShowWhitespaces|</v>
       </c>
       <c r="H127" t="s">
         <v>366</v>
@@ -8620,8 +8622,8 @@
         <v>876</v>
       </c>
       <c r="G128" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.WordDeleteToEnd|EditorDeleteToWordEnd</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.WordDeleteToEnd|EditorDeleteToWordEnd|</v>
       </c>
       <c r="H128" t="s">
         <v>369</v>
@@ -8648,8 +8650,8 @@
         <v>875</v>
       </c>
       <c r="G129" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.WordDeleteToStart|EditorDeleteToWordStart</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.WordDeleteToStart|EditorDeleteToWordStart|</v>
       </c>
       <c r="H129" t="s">
         <v>372</v>
@@ -8676,8 +8678,8 @@
         <v>1178</v>
       </c>
       <c r="G130" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Manipulation Shortcut Keys|Edit.WordTranspose|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.WordTranspose|N/A|</v>
       </c>
       <c r="H130" t="s">
         <v>375</v>
@@ -8704,8 +8706,8 @@
         <v>818</v>
       </c>
       <c r="G131" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.CharLeft|EditorLeft</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.CharLeft|EditorLeft|</v>
       </c>
       <c r="H131" t="s">
         <v>379</v>
@@ -8732,8 +8734,8 @@
         <v>819</v>
       </c>
       <c r="G132" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.CharRight|EditorRight</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.CharRight|EditorRight|</v>
       </c>
       <c r="H132" t="s">
         <v>382</v>
@@ -8760,8 +8762,8 @@
         <v>883</v>
       </c>
       <c r="G133" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.DocumentEnd|EditorTextEnd</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.DocumentEnd|EditorTextEnd|</v>
       </c>
       <c r="H133" t="s">
         <v>385</v>
@@ -8788,8 +8790,8 @@
         <v>884</v>
       </c>
       <c r="G134" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.DocumentStart|EditorTextStart</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.DocumentStart|EditorTextStart|</v>
       </c>
       <c r="H134" t="s">
         <v>388</v>
@@ -8816,8 +8818,8 @@
         <v>873</v>
       </c>
       <c r="G135" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.GoTo|GotoLine</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.GoTo|GotoLine|</v>
       </c>
       <c r="H135" t="s">
         <v>391</v>
@@ -8844,8 +8846,8 @@
         <v>1178</v>
       </c>
       <c r="G136" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.GotoBrace|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.GotoBrace|N/A|</v>
       </c>
       <c r="H136" t="s">
         <v>394</v>
@@ -8872,8 +8874,8 @@
         <v>877</v>
       </c>
       <c r="G137" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.LineDown|EditorDown</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineDown|EditorDown|</v>
       </c>
       <c r="H137" t="s">
         <v>397</v>
@@ -8900,8 +8902,8 @@
         <v>636</v>
       </c>
       <c r="G138" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.LineEnd|EditorLineEnd</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineEnd|EditorLineEnd|</v>
       </c>
       <c r="H138" t="s">
         <v>400</v>
@@ -8928,8 +8930,8 @@
         <v>635</v>
       </c>
       <c r="G139" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.LineStart|EditorLineStart</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineStart|EditorLineStart|</v>
       </c>
       <c r="H139" t="s">
         <v>403</v>
@@ -8956,8 +8958,8 @@
         <v>878</v>
       </c>
       <c r="G140" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.LineUp|EditorUp</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineUp|EditorUp|</v>
       </c>
       <c r="H140" t="s">
         <v>406</v>
@@ -8984,8 +8986,8 @@
         <v>863</v>
       </c>
       <c r="G141" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.NextBookmark|GotoNextBookmark</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.NextBookmark|GotoNextBookmark|</v>
       </c>
       <c r="H141" t="s">
         <v>409</v>
@@ -9012,8 +9014,8 @@
         <v>821</v>
       </c>
       <c r="G142" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.PageDown|EditorPageDown</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.PageDown|EditorPageDown|</v>
       </c>
       <c r="H142" t="s">
         <v>412</v>
@@ -9040,8 +9042,8 @@
         <v>820</v>
       </c>
       <c r="G143" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.PageUp|EditorPageUp</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.PageUp|EditorPageUp|</v>
       </c>
       <c r="H143" t="s">
         <v>415</v>
@@ -9068,8 +9070,8 @@
         <v>864</v>
       </c>
       <c r="G144" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.PreviousBookmark|GotoPreviousBookmark</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.PreviousBookmark|GotoPreviousBookmark|</v>
       </c>
       <c r="H144" t="s">
         <v>418</v>
@@ -9096,8 +9098,8 @@
         <v>1178</v>
       </c>
       <c r="G145" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.QuickInfo|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.QuickInfo|N/A|</v>
       </c>
       <c r="H145" t="s">
         <v>421</v>
@@ -9124,8 +9126,8 @@
         <v>902</v>
       </c>
       <c r="G146" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.ScrollLineDown|EditorScrollDown</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.ScrollLineDown|EditorScrollDown|</v>
       </c>
       <c r="H146" t="s">
         <v>424</v>
@@ -9152,8 +9154,8 @@
         <v>903</v>
       </c>
       <c r="G147" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.ScrollLineUp|EditorScrollUp</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.ScrollLineUp|EditorScrollUp|</v>
       </c>
       <c r="H147" t="s">
         <v>427</v>
@@ -9177,8 +9179,8 @@
         <v>0</v>
       </c>
       <c r="G148" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.ShowTileGrid|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.ShowTileGrid||</v>
       </c>
       <c r="H148" t="s">
         <v>430</v>
@@ -9205,8 +9207,8 @@
         <v>892</v>
       </c>
       <c r="G149" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.WordNext|EditorNextWord</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.WordNext|EditorNextWord|</v>
       </c>
       <c r="H149" t="s">
         <v>433</v>
@@ -9233,8 +9235,8 @@
         <v>891</v>
       </c>
       <c r="G150" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|Edit.WordPrevious|EditorPreviousWord</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.WordPrevious|EditorPreviousWord|</v>
       </c>
       <c r="H150" t="s">
         <v>436</v>
@@ -9259,8 +9261,8 @@
       </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|View.BrowseNext|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|View.BrowseNext||</v>
       </c>
       <c r="H151" t="s">
         <v>438</v>
@@ -9285,8 +9287,8 @@
       </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Navigation Shortcut Keys|View.BrowsePrevious|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|View.BrowsePrevious||</v>
       </c>
       <c r="H152" t="s">
         <v>440</v>
@@ -9313,8 +9315,8 @@
         <v>880</v>
       </c>
       <c r="G153" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.CharLeftExtend|EditorLeftWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharLeftExtend|EditorLeftWithSelection|</v>
       </c>
       <c r="H153" t="s">
         <v>446</v>
@@ -9338,8 +9340,8 @@
         <v>0</v>
       </c>
       <c r="G154" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.CharLeftExtendColumn|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharLeftExtendColumn||</v>
       </c>
       <c r="H154" t="s">
         <v>449</v>
@@ -9366,8 +9368,8 @@
         <v>881</v>
       </c>
       <c r="G155" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.CharRightExtend|EditorRightWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharRightExtend|EditorRightWithSelection|</v>
       </c>
       <c r="H155" t="s">
         <v>452</v>
@@ -9391,8 +9393,8 @@
         <v>0</v>
       </c>
       <c r="G156" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.CharRightExtendColumn|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharRightExtendColumn||</v>
       </c>
       <c r="H156" t="s">
         <v>455</v>
@@ -9419,8 +9421,8 @@
         <v>885</v>
       </c>
       <c r="G157" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.DocumentEndExtend|EditorTextEndWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.DocumentEndExtend|EditorTextEndWithSelection|</v>
       </c>
       <c r="H157" t="s">
         <v>458</v>
@@ -9447,8 +9449,8 @@
         <v>886</v>
       </c>
       <c r="G158" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.DocumentStartExtend|EditorTextStartWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.DocumentStartExtend|EditorTextStartWithSelection|</v>
       </c>
       <c r="H158" t="s">
         <v>461</v>
@@ -9472,8 +9474,8 @@
         <v>0</v>
       </c>
       <c r="G159" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.GotoBraceExtend|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.GotoBraceExtend||</v>
       </c>
       <c r="H159" t="s">
         <v>464</v>
@@ -9500,8 +9502,8 @@
         <v>882</v>
       </c>
       <c r="G160" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineDownExtend|EditorDownWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineDownExtend|EditorDownWithSelection|</v>
       </c>
       <c r="H160" t="s">
         <v>467</v>
@@ -9528,8 +9530,8 @@
         <v>909</v>
       </c>
       <c r="G161" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineDownExtendColumn|MoveLineDown</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineDownExtendColumn|MoveLineDown|</v>
       </c>
       <c r="H161" t="s">
         <v>470</v>
@@ -9556,8 +9558,8 @@
         <v>887</v>
       </c>
       <c r="G162" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineEndExtend|EditorLineEndWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineEndExtend|EditorLineEndWithSelection|</v>
       </c>
       <c r="H162" t="s">
         <v>473</v>
@@ -9581,8 +9583,8 @@
         <v>0</v>
       </c>
       <c r="G163" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineEndExtendColumn|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineEndExtendColumn||</v>
       </c>
       <c r="H163" t="s">
         <v>476</v>
@@ -9609,8 +9611,8 @@
         <v>888</v>
       </c>
       <c r="G164" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineStartExtend|EditorLineStartWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineStartExtend|EditorLineStartWithSelection|</v>
       </c>
       <c r="H164" t="s">
         <v>479</v>
@@ -9634,14 +9636,14 @@
         <v>0</v>
       </c>
       <c r="G165" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineStartExtendColumn|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineStartExtendColumn||</v>
       </c>
       <c r="H165" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>521</v>
       </c>
@@ -9662,8 +9664,8 @@
         <v>901</v>
       </c>
       <c r="G166" s="1" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineUpExtend|EditorUpWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineUpExtend|EditorUpWithSelection|</v>
       </c>
       <c r="H166" t="s">
         <v>484</v>
@@ -9690,8 +9692,8 @@
         <v>908</v>
       </c>
       <c r="G167" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.LineUpExtendColumn|MoveLineUp</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineUpExtendColumn|MoveLineUp|</v>
       </c>
       <c r="H167" t="s">
         <v>487</v>
@@ -9718,8 +9720,8 @@
         <v>897</v>
       </c>
       <c r="G168" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.PageDownExtend|EditorPageDownWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.PageDownExtend|EditorPageDownWithSelection|</v>
       </c>
       <c r="H168" t="s">
         <v>490</v>
@@ -9746,8 +9748,8 @@
         <v>898</v>
       </c>
       <c r="G169" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.PageUpExtend|EditorPageUpWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.PageUpExtend|EditorPageUpWithSelection|</v>
       </c>
       <c r="H169" t="s">
         <v>493</v>
@@ -9774,8 +9776,8 @@
         <v>627</v>
       </c>
       <c r="G170" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.SelectAll|$SelectAll</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.SelectAll|$SelectAll|</v>
       </c>
       <c r="H170" t="s">
         <v>496</v>
@@ -9802,8 +9804,8 @@
         <v>1179</v>
       </c>
       <c r="G171" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.SelectCurrentWord|EditorSelectWord</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.SelectCurrentWord|EditorSelectWord|</v>
       </c>
       <c r="H171" t="s">
         <v>499</v>
@@ -9830,8 +9832,8 @@
         <v>1178</v>
       </c>
       <c r="G172" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.SelectToLastGoBack|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.SelectToLastGoBack|N/A|</v>
       </c>
       <c r="H172" t="s">
         <v>502</v>
@@ -9858,8 +9860,8 @@
         <v>896</v>
       </c>
       <c r="G173" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.ViewBottomExtend|EditorMoveToPageBottomWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.ViewBottomExtend|EditorMoveToPageBottomWithSelection|</v>
       </c>
       <c r="H173" t="s">
         <v>505</v>
@@ -9886,8 +9888,8 @@
         <v>895</v>
       </c>
       <c r="G174" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.ViewTopExtend|EditorMoveToPageTopWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.ViewTopExtend|EditorMoveToPageTopWithSelection|</v>
       </c>
       <c r="H174" t="s">
         <v>508</v>
@@ -9914,8 +9916,8 @@
         <v>894</v>
       </c>
       <c r="G175" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.WordNextExtend|EditorNextWordWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordNextExtend|EditorNextWordWithSelection|</v>
       </c>
       <c r="H175" t="s">
         <v>511</v>
@@ -9942,8 +9944,8 @@
         <v>911</v>
       </c>
       <c r="G176" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.WordNextExtendColumn|MoveElementRight</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordNextExtendColumn|MoveElementRight|</v>
       </c>
       <c r="H176" t="s">
         <v>514</v>
@@ -9970,8 +9972,8 @@
         <v>893</v>
       </c>
       <c r="G177" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.WordPreviousExtend|EditorPreviousWordWithSelection</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordPreviousExtend|EditorPreviousWordWithSelection|</v>
       </c>
       <c r="H177" t="s">
         <v>517</v>
@@ -9998,8 +10000,8 @@
         <v>910</v>
       </c>
       <c r="G178" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Text Selection Shortcut Keys|Edit.WordPreviousExtendColumn|MoveElementLeft</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordPreviousExtendColumn|MoveElementLeft|</v>
       </c>
       <c r="H178" t="s">
         <v>520</v>
@@ -10023,8 +10025,8 @@
         <v>0</v>
       </c>
       <c r="G179" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|Tools.CommandWindowMarkMode|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|Tools.CommandWindowMarkMode||</v>
       </c>
       <c r="H179" t="s">
         <v>609</v>
@@ -10051,8 +10053,8 @@
         <v>832</v>
       </c>
       <c r="G180" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.ClassView|ActivateHierarchyToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.ClassView|ActivateHierarchyToolWindow|</v>
       </c>
       <c r="H180" t="s">
         <v>525</v>
@@ -10079,8 +10081,8 @@
         <v>840</v>
       </c>
       <c r="G181" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.CommandWindow|IdeScriptingConsole</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.CommandWindow|IdeScriptingConsole|</v>
       </c>
       <c r="H181" t="s">
         <v>619</v>
@@ -10107,8 +10109,8 @@
         <v>827</v>
       </c>
       <c r="G182" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.DocumentOutline|ActivateStructureToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.DocumentOutline|ActivateStructureToolWindow|</v>
       </c>
       <c r="H182" t="s">
         <v>529</v>
@@ -10135,14 +10137,14 @@
         <v>826</v>
       </c>
       <c r="G183" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.Favorites|ActivateFavoritesToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.Favorites|ActivateFavoritesToolWindow|</v>
       </c>
       <c r="H183" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>553</v>
       </c>
@@ -10163,8 +10165,8 @@
         <v>828</v>
       </c>
       <c r="G184" s="1" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.Output|ActivateRunToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.Output|ActivateRunToolWindow|</v>
       </c>
       <c r="H184" t="s">
         <v>533</v>
@@ -10191,8 +10193,8 @@
         <v>1178</v>
       </c>
       <c r="G185" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.PropertiesWindow|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.PropertiesWindow|N/A|</v>
       </c>
       <c r="H185" t="s">
         <v>536</v>
@@ -10216,8 +10218,8 @@
         <v>0</v>
       </c>
       <c r="G186" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.ResourceView|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.ResourceView||</v>
       </c>
       <c r="H186" t="s">
         <v>539</v>
@@ -10244,8 +10246,8 @@
         <v>842</v>
       </c>
       <c r="G187" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.ServerExplorer|ActivateDatabaseToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.ServerExplorer|ActivateDatabaseToolWindow|</v>
       </c>
       <c r="H187" t="s">
         <v>542</v>
@@ -10272,8 +10274,8 @@
         <v>833</v>
       </c>
       <c r="G188" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.SolutionExplorer|ActivateProjectToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.SolutionExplorer|ActivateProjectToolWindow|</v>
       </c>
       <c r="H188" t="s">
         <v>551</v>
@@ -10300,8 +10302,8 @@
         <v>841</v>
       </c>
       <c r="G189" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.TaskList|ActivateTODOToolWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.TaskList|ActivateTODOToolWindow|</v>
       </c>
       <c r="H189" t="s">
         <v>620</v>
@@ -10328,8 +10330,8 @@
         <v>1178</v>
       </c>
       <c r="G190" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Tool Window Shortcut Keys|View.Toolbox|N/A</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.Toolbox|N/A|</v>
       </c>
       <c r="H190" t="s">
         <v>549</v>
@@ -10356,8 +10358,8 @@
         <v>843</v>
       </c>
       <c r="G191" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|View.FullScreen|ToggleFullScreen</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|View.FullScreen|ToggleFullScreen|</v>
       </c>
       <c r="H191" t="s">
         <v>556</v>
@@ -10384,8 +10386,8 @@
         <v>830</v>
       </c>
       <c r="G192" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|View.NavigateBackward|Back</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|View.NavigateBackward|Back|</v>
       </c>
       <c r="H192" t="s">
         <v>559</v>
@@ -10412,8 +10414,8 @@
         <v>831</v>
       </c>
       <c r="G193" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|View.NavigateForward|Forward</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|View.NavigateForward|Forward|</v>
       </c>
       <c r="H193" t="s">
         <v>562</v>
@@ -10440,8 +10442,8 @@
         <v>834</v>
       </c>
       <c r="G194" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.ActivateDocumentWindow|FocusEditor</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.ActivateDocumentWindow|FocusEditor|</v>
       </c>
       <c r="H194" t="s">
         <v>29</v>
@@ -10468,8 +10470,8 @@
         <v>845</v>
       </c>
       <c r="G195" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.CloseDocumentWindow|CloseContent</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.CloseDocumentWindow|CloseContent|</v>
       </c>
       <c r="H195" t="s">
         <v>567</v>
@@ -10496,8 +10498,8 @@
         <v>844</v>
       </c>
       <c r="G196" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.CloseToolWindow|HideActiveWindow</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.CloseToolWindow|HideActiveWindow|</v>
       </c>
       <c r="H196" t="s">
         <v>570</v>
@@ -10524,8 +10526,8 @@
         <v>848</v>
       </c>
       <c r="G197" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.NextDocumentWindow|NextTab</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextDocumentWindow|NextTab|</v>
       </c>
       <c r="H197" t="s">
         <v>573</v>
@@ -10552,8 +10554,8 @@
         <v>846</v>
       </c>
       <c r="G198" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.NextPane|NextSplitter</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextPane|NextSplitter|</v>
       </c>
       <c r="H198" t="s">
         <v>576</v>
@@ -10580,8 +10582,8 @@
         <v>846</v>
       </c>
       <c r="G199" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.NextSplitPane|NextSplitter</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextSplitPane|NextSplitter|</v>
       </c>
       <c r="H199" t="s">
         <v>579</v>
@@ -10608,8 +10610,8 @@
         <v>848</v>
       </c>
       <c r="G200" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.NextTab|NextTab</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextTab|NextTab|</v>
       </c>
       <c r="H200" t="s">
         <v>582</v>
@@ -10636,8 +10638,8 @@
         <v>849</v>
       </c>
       <c r="G201" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.PreviousDocumentWindow|PreviousTab</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousDocumentWindow|PreviousTab|</v>
       </c>
       <c r="H201" t="s">
         <v>585</v>
@@ -10664,8 +10666,8 @@
         <v>847</v>
       </c>
       <c r="G202" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.PreviousPane|PrevSplitter</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousPane|PrevSplitter|</v>
       </c>
       <c r="H202" t="s">
         <v>588</v>
@@ -10692,8 +10694,8 @@
         <v>847</v>
       </c>
       <c r="G203" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.PreviousSplitPane|PrevSplitter</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousSplitPane|PrevSplitter|</v>
       </c>
       <c r="H203" t="s">
         <v>591</v>
@@ -10720,8 +10722,8 @@
         <v>849</v>
       </c>
       <c r="G204" t="str">
-        <f>Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]]</f>
-        <v>Window Management Shortcut Keys|Window.PreviousTab|PreviousTab</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousTab|PreviousTab|</v>
       </c>
       <c r="H204" t="s">
         <v>594</v>

</xml_diff>

<commit_message>
Add keystrokes to readme.
</commit_message>
<xml_diff>
--- a/WellEngineered.us VC++ 6.0 Shortcuts.xlsx
+++ b/WellEngineered.us VC++ 6.0 Shortcuts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D53B95E-78D2-4CD9-A8D8-DF3BC048471E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C251C19-26E1-45A1-814C-0858D098A1CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5D8658FC-F053-4B4D-BC9B-4C701ADA3E99}"/>
   </bookViews>
@@ -4789,7 +4789,7 @@
     </tableColumn>
     <tableColumn id="7" xr3:uid="{AD3AB443-69FC-4ED6-9DE9-F3E9E01AD994}" name="IDEA_Keymap_ID"/>
     <tableColumn id="8" xr3:uid="{9C6E70BC-6004-42BB-8E99-008FFF3A215B}" name="Column1" dataDxfId="0">
-      <calculatedColumnFormula>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</calculatedColumnFormula>
+      <calculatedColumnFormula>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{4EBEDB49-82CC-456A-8155-4D2F3CD27D4E}" name="Description"/>
   </tableColumns>
@@ -5096,7 +5096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D07097-255A-46B5-AC8C-91A030E6460F}">
   <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -5107,7 +5107,7 @@
     <col min="4" max="4" width="49.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="114" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="222.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="122" bestFit="1" customWidth="1"/>
   </cols>
@@ -5159,8 +5159,8 @@
         <v>1178</v>
       </c>
       <c r="G2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.ApplyCodeChanges|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ApplyCodeChanges|N/A|ALT F10|</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>67</v>
@@ -5187,8 +5187,8 @@
         <v>1178</v>
       </c>
       <c r="G3" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Autos|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Autos|N/A|CONTROL ALT V, A|</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>70</v>
@@ -5215,8 +5215,8 @@
         <v>871</v>
       </c>
       <c r="G4" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.BreakAll|Pause|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.BreakAll|Pause|CONTROL ALT BREAK|</v>
       </c>
       <c r="H4" t="s">
         <v>73</v>
@@ -5243,8 +5243,8 @@
         <v>837</v>
       </c>
       <c r="G5" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Breakpoints|ViewBreakpoints|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Breakpoints|ViewBreakpoints|ALT F9 || CONTROL ALT B|</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>76</v>
@@ -5271,8 +5271,8 @@
         <v>1178</v>
       </c>
       <c r="G6" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.CallStack|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.CallStack|N/A|ALT 7 || CONTROL ALT C|</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>79</v>
@@ -5299,8 +5299,8 @@
         <v>1040</v>
       </c>
       <c r="G7" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.ClearAllBreakpoints|RiderRemoveAllLineBreakpoints|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ClearAllBreakpoints|RiderRemoveAllLineBreakpoints|CONTROL SHIFT F9|</v>
       </c>
       <c r="H7" t="s">
         <v>82</v>
@@ -5327,8 +5327,8 @@
         <v>851</v>
       </c>
       <c r="G8" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Continue ***|Resume|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Continue ***|Resume|F5|</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -5353,8 +5353,8 @@
         <v>858</v>
       </c>
       <c r="G9" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Disassembly|ActivateILViewerToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Disassembly|ActivateILViewerToolWindow|ALT 8|</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>85</v>
@@ -5381,8 +5381,8 @@
         <v>853</v>
       </c>
       <c r="G10" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.EnableBreakpoint|ToggleBreakpointEnabled|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.EnableBreakpoint|ToggleBreakpointEnabled|CONTROL F9|</v>
       </c>
       <c r="H10" t="s">
         <v>88</v>
@@ -5409,8 +5409,8 @@
         <v>1490</v>
       </c>
       <c r="G11" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Exceptions|OpenExceptionSettings|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Exceptions|OpenExceptionSettings|CONTROL ALT E|</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>91</v>
@@ -5437,8 +5437,8 @@
         <v>1491</v>
       </c>
       <c r="G12" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Immediate|NavigateToImmediateWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Immediate|NavigateToImmediateWindow|CONTROL ALT I|</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>610</v>
@@ -5465,8 +5465,8 @@
         <v>1178</v>
       </c>
       <c r="G13" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Locals|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Locals|N/A|ALT 4 || CONTROL ALT V, L|</v>
       </c>
       <c r="H13" t="s">
         <v>95</v>
@@ -5493,8 +5493,8 @@
         <v>1178</v>
       </c>
       <c r="G14" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Memory1|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory1|N/A|ALT 6 || CONTROL ALT M, 1|</v>
       </c>
       <c r="H14" t="s">
         <v>98</v>
@@ -5521,8 +5521,8 @@
         <v>1178</v>
       </c>
       <c r="G15" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Memory2|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory2|N/A|CONTROL ALT M, 2|</v>
       </c>
       <c r="H15" t="s">
         <v>101</v>
@@ -5549,8 +5549,8 @@
         <v>1178</v>
       </c>
       <c r="G16" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Memory3|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory3|N/A|CONTROL ALT M, 3|</v>
       </c>
       <c r="H16" t="s">
         <v>104</v>
@@ -5577,8 +5577,8 @@
         <v>1178</v>
       </c>
       <c r="G17" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Memory4|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Memory4|N/A|CONTROL ALT M, 4|</v>
       </c>
       <c r="H17" t="s">
         <v>107</v>
@@ -5605,8 +5605,8 @@
         <v>1178</v>
       </c>
       <c r="G18" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Modules|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Modules|N/A|CONTROL ALT U|</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>110</v>
@@ -5633,8 +5633,8 @@
         <v>855</v>
       </c>
       <c r="G19" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.NewBreakpoint|ToggleTemporaryLineBreakpoint|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.NewBreakpoint|ToggleTemporaryLineBreakpoint|CONTROL B|</v>
       </c>
       <c r="H19" t="s">
         <v>113</v>
@@ -5661,8 +5661,8 @@
         <v>1178</v>
       </c>
       <c r="G20" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.QuickWatch|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.QuickWatch|N/A|CONTROL ALT Q || SHIFT F9|</v>
       </c>
       <c r="H20" t="s">
         <v>611</v>
@@ -5689,8 +5689,8 @@
         <v>1178</v>
       </c>
       <c r="G21" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Registers|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Registers|N/A|ALT 5 || CONTROL ALT G|</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>118</v>
@@ -5717,8 +5717,8 @@
         <v>1178</v>
       </c>
       <c r="G22" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Restart|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Restart|N/A|CONTROL SHIFT F5|</v>
       </c>
       <c r="H22" t="s">
         <v>121</v>
@@ -5745,8 +5745,8 @@
         <v>1178</v>
       </c>
       <c r="G23" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.RunningDocuments|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.RunningDocuments|N/A|CONTROL ALT N|</v>
       </c>
       <c r="H23" t="s">
         <v>124</v>
@@ -5773,8 +5773,8 @@
         <v>857</v>
       </c>
       <c r="G24" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.RunToCursor|RunToCursor|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.RunToCursor|RunToCursor|CONTROL F10|</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>127</v>
@@ -5801,8 +5801,8 @@
         <v>1178</v>
       </c>
       <c r="G25" s="2" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.SetNextStatement|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.SetNextStatement|N/A|CONTROL SHIFT F10|</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>130</v>
@@ -5829,8 +5829,8 @@
         <v>854</v>
       </c>
       <c r="G26" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.ShowNextStatement|ShowExecutionPoint|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ShowNextStatement|ShowExecutionPoint|ALT num*|</v>
       </c>
       <c r="H26" t="s">
         <v>133</v>
@@ -5857,8 +5857,8 @@
         <v>872</v>
       </c>
       <c r="G27" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Start (Continue)|#|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Start (Continue)|#|F5|</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>135</v>
@@ -5885,8 +5885,8 @@
         <v>850</v>
       </c>
       <c r="G28" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Start ***|Debug|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Start ***|Debug|ALT F5|</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -5911,8 +5911,8 @@
         <v>856</v>
       </c>
       <c r="G29" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.StartWithoutDebugging|Run|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StartWithoutDebugging|Run|CONTROL F5|</v>
       </c>
       <c r="H29" t="s">
         <v>138</v>
@@ -5939,8 +5939,8 @@
         <v>859</v>
       </c>
       <c r="G30" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.StepInto|StepInto|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StepInto|StepInto|F11|</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>141</v>
@@ -5967,8 +5967,8 @@
         <v>860</v>
       </c>
       <c r="G31" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.StepOut|StepOut|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StepOut|StepOut|SHIFT F11|</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>144</v>
@@ -5995,8 +5995,8 @@
         <v>861</v>
       </c>
       <c r="G32" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.StepOver|StepOver|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StepOver|StepOver|F10|</v>
       </c>
       <c r="H32" t="s">
         <v>147</v>
@@ -6023,8 +6023,8 @@
         <v>862</v>
       </c>
       <c r="G33" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.StopDebugging|Stop|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.StopDebugging|Stop|SHIFT F5|</v>
       </c>
       <c r="H33" t="s">
         <v>150</v>
@@ -6051,8 +6051,8 @@
         <v>1178</v>
       </c>
       <c r="G34" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.This|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.This|N/A|CONTROL ALT V, T|</v>
       </c>
       <c r="H34" t="s">
         <v>153</v>
@@ -6079,8 +6079,8 @@
         <v>1178</v>
       </c>
       <c r="G35" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.Threads|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.Threads|N/A|CONTROL ALT H|</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>156</v>
@@ -6107,8 +6107,8 @@
         <v>852</v>
       </c>
       <c r="G36" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.ToggleBreakpoint|ToggleLineBreakpoint|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ToggleBreakpoint|ToggleLineBreakpoint|F9|</v>
       </c>
       <c r="H36" t="s">
         <v>159</v>
@@ -6135,8 +6135,8 @@
         <v>1178</v>
       </c>
       <c r="G37" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Debug.ToggleDisassembly|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Debug.ToggleDisassembly|N/A|CONTROL F11|</v>
       </c>
       <c r="H37" t="s">
         <v>162</v>
@@ -6163,8 +6163,8 @@
         <v>836</v>
       </c>
       <c r="G38" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Debug Shortcut Keys|Tools.DebugProcesses|XDebugger.AttachToProcess|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Debug Shortcut Keys|Tools.DebugProcesses|XDebugger.AttachToProcess|CONTROL ALT P|</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>165</v>
@@ -6191,8 +6191,8 @@
         <v>622</v>
       </c>
       <c r="G39" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.Copy|$Copy|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Copy|$Copy|CONTROL INSERT || CONTROL C|</v>
       </c>
       <c r="H39" t="s">
         <v>4</v>
@@ -6219,8 +6219,8 @@
         <v>623</v>
       </c>
       <c r="G40" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.Cut|$Cut|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Cut|$Cut|SHIFT DELETE || CONTROL X|</v>
       </c>
       <c r="H40" t="s">
         <v>7</v>
@@ -6247,8 +6247,8 @@
         <v>1178</v>
       </c>
       <c r="G41" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.CycleClipboardRing|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.CycleClipboardRing|N/A|CONTROL SHIFT V || CONTROL SHIFT INSERT|</v>
       </c>
       <c r="H41" t="s">
         <v>7</v>
@@ -6275,8 +6275,8 @@
         <v>1181</v>
       </c>
       <c r="G42" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.GotoNextLocation|GotoNextError|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.GotoNextLocation|GotoNextError|F8|</v>
       </c>
       <c r="H42" t="s">
         <v>63</v>
@@ -6303,8 +6303,8 @@
         <v>1182</v>
       </c>
       <c r="G43" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.GotoPreviousLocation|GotoPreviousError|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.GotoPreviousLocation|GotoPreviousError|SHIFT F8|</v>
       </c>
       <c r="H43" t="s">
         <v>17</v>
@@ -6328,8 +6328,8 @@
         <v>0</v>
       </c>
       <c r="G44" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.GoToReference||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.GoToReference||SHIFT F12|</v>
       </c>
       <c r="H44" t="s">
         <v>20</v>
@@ -6353,8 +6353,8 @@
         <v>0</v>
       </c>
       <c r="G45" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.ListMembers||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.ListMembers||CONTROL ALT T|</v>
       </c>
       <c r="H45" t="s">
         <v>12</v>
@@ -6381,8 +6381,8 @@
         <v>624</v>
       </c>
       <c r="G46" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.Paste|$Paste|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Paste|$Paste|CONTROL V || SHIFT INSERT|</v>
       </c>
       <c r="H46" t="s">
         <v>23</v>
@@ -6409,8 +6409,8 @@
         <v>625</v>
       </c>
       <c r="G47" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.Redo|$Redo|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Redo|$Redo|CONTROL Y || CONTROL SHIFT Z || SHIFT ALT BACKSPACE|</v>
       </c>
       <c r="H47" t="s">
         <v>26</v>
@@ -6437,8 +6437,8 @@
         <v>637</v>
       </c>
       <c r="G48" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.SelectionCancel|EditorEscape|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.SelectionCancel|EditorEscape|ESC|</v>
       </c>
       <c r="H48" t="s">
         <v>29</v>
@@ -6465,8 +6465,8 @@
         <v>626</v>
       </c>
       <c r="G49" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Edit.Undo|$Undo|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Edit.Undo|$Undo|CONTROL Z || ALT BACKSPACE|</v>
       </c>
       <c r="H49" t="s">
         <v>32</v>
@@ -6493,8 +6493,8 @@
         <v>838</v>
       </c>
       <c r="G50" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|File.Print|Print|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|File.Print|Print|CONTROL P|</v>
       </c>
       <c r="H50" t="s">
         <v>35</v>
@@ -6521,8 +6521,8 @@
         <v>835</v>
       </c>
       <c r="G51" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|File.SaveAll|SaveAll|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|File.SaveAll|SaveAll|CONTROL SHIFT S|</v>
       </c>
       <c r="H51" t="s">
         <v>38</v>
@@ -6549,8 +6549,8 @@
         <v>839</v>
       </c>
       <c r="G52" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|File.SaveSelectedItems|SaveDocument|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|File.SaveSelectedItems|SaveDocument|CONTROL S|</v>
       </c>
       <c r="H52" t="s">
         <v>41</v>
@@ -6577,8 +6577,8 @@
         <v>1178</v>
       </c>
       <c r="G53" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|Tools.GoToCommandLine|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|Tools.GoToCommandLine|N/A|CONTROL /|</v>
       </c>
       <c r="H53" t="s">
         <v>613</v>
@@ -6602,8 +6602,8 @@
         <v>0</v>
       </c>
       <c r="G54" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.NextTask||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.NextTask||F4 || CONTROL SHIFT F12|</v>
       </c>
       <c r="H54" t="s">
         <v>45</v>
@@ -6627,8 +6627,8 @@
         <v>0</v>
       </c>
       <c r="G55" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.PopBrowseContext||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.PopBrowseContext||CONTROL num*|</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>64</v>
@@ -6652,8 +6652,8 @@
         <v>0</v>
       </c>
       <c r="G56" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.PreviousTask||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.PreviousTask||SHIFT F4|</v>
       </c>
       <c r="H56" t="s">
         <v>50</v>
@@ -6680,8 +6680,8 @@
         <v>1178</v>
       </c>
       <c r="G57" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.ViewCode|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.ViewCode|N/A|CONTROL ALT 0|</v>
       </c>
       <c r="H57" t="s">
         <v>53</v>
@@ -6708,8 +6708,8 @@
         <v>1178</v>
       </c>
       <c r="G58" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.ViewDesigner|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.ViewDesigner|N/A|SHIFT F7|</v>
       </c>
       <c r="H58" t="s">
         <v>56</v>
@@ -6736,8 +6736,8 @@
         <v>830</v>
       </c>
       <c r="G59" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.WebNavigateBack|Back|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.WebNavigateBack|Back|ALT LEFT_ARROW|</v>
       </c>
       <c r="H59" t="s">
         <v>59</v>
@@ -6764,8 +6764,8 @@
         <v>831</v>
       </c>
       <c r="G60" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Global Shortcut Keys|View.WebNavigateForward|Forward|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Global Shortcut Keys|View.WebNavigateForward|Forward|ALT RIGHT_ARROW|</v>
       </c>
       <c r="H60" t="s">
         <v>62</v>
@@ -6792,8 +6792,8 @@
         <v>1338</v>
       </c>
       <c r="G61" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|Edit.FindSymbol|GotoSymbol|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|Edit.FindSymbol|GotoSymbol|ALT F12 || CONTROL SHIFT Y|</v>
       </c>
       <c r="H61" t="s">
         <v>271</v>
@@ -6817,8 +6817,8 @@
         <v>0</v>
       </c>
       <c r="G62" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|Edit.GoToDeclaration||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|Edit.GoToDeclaration||CONTROL F12 || CONTROL ALT F12|</v>
       </c>
       <c r="H62" t="s">
         <v>256</v>
@@ -6845,8 +6845,8 @@
         <v>1180</v>
       </c>
       <c r="G63" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|Edit.GoToDefinition|GotoDeclaration|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|Edit.GoToDefinition|GotoDeclaration|F12|</v>
       </c>
       <c r="H63" t="s">
         <v>259</v>
@@ -6870,8 +6870,8 @@
         <v>0</v>
       </c>
       <c r="G64" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|View.FindSymbolResults||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.FindSymbolResults||CONTROL ALT Y|</v>
       </c>
       <c r="H64" t="s">
         <v>272</v>
@@ -6898,8 +6898,8 @@
         <v>1178</v>
       </c>
       <c r="G65" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|View.ObjectBrowser|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.ObjectBrowser|N/A|CONTROL ALT J|</v>
       </c>
       <c r="H65" t="s">
         <v>264</v>
@@ -6926,8 +6926,8 @@
         <v>1178</v>
       </c>
       <c r="G66" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|View.ObjectBrowserBack|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.ObjectBrowserBack|N/A|ALT -|</v>
       </c>
       <c r="H66" t="s">
         <v>267</v>
@@ -6951,8 +6951,8 @@
         <v>0</v>
       </c>
       <c r="G67" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Object Browser Shortcut Keys|View.ObjectBrowserForward||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Object Browser Shortcut Keys|View.ObjectBrowserForward||SHIFT ALT -|</v>
       </c>
       <c r="H67" t="s">
         <v>270</v>
@@ -6979,8 +6979,8 @@
         <v>865</v>
       </c>
       <c r="G68" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|Build.BuildSolution|BuildSolutionAction|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|Build.BuildSolution|BuildSolutionAction|F7|</v>
       </c>
       <c r="H68" t="s">
         <v>168</v>
@@ -7007,8 +7007,8 @@
         <v>866</v>
       </c>
       <c r="G69" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|Build.Cancel|CancelBuildAction|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|Build.Cancel|CancelBuildAction|CONTROL BREAK|</v>
       </c>
       <c r="H69" t="s">
         <v>171</v>
@@ -7035,8 +7035,8 @@
         <v>867</v>
       </c>
       <c r="G70" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|Build.Compile|RebuildSolutionAction|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|Build.Compile|RebuildSolutionAction|CONTROL F7|</v>
       </c>
       <c r="H70" t="s">
         <v>174</v>
@@ -7060,8 +7060,8 @@
         <v>0</v>
       </c>
       <c r="G71" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|File.AddExistingItem||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|File.AddExistingItem||SHIFT ALT A|</v>
       </c>
       <c r="H71" t="s">
         <v>189</v>
@@ -7085,8 +7085,8 @@
         <v>0</v>
       </c>
       <c r="G72" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|File.AddNewItem||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|File.AddNewItem||CONTROL SHIFT A|</v>
       </c>
       <c r="H72" t="s">
         <v>192</v>
@@ -7113,8 +7113,8 @@
         <v>869</v>
       </c>
       <c r="G73" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|File.NewFile|NewElement|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|File.NewFile|NewElement|CONTROL N|</v>
       </c>
       <c r="H73" t="s">
         <v>177</v>
@@ -7141,8 +7141,8 @@
         <v>989</v>
       </c>
       <c r="G74" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|File.NewProject|NewProject|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|File.NewProject|NewProject|CONTROL SHIFT N|</v>
       </c>
       <c r="H74" t="s">
         <v>180</v>
@@ -7169,8 +7169,8 @@
         <v>870</v>
       </c>
       <c r="G75" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|File.OpenFile|OpenFile|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|File.OpenFile|OpenFile|CONTROL O|</v>
       </c>
       <c r="H75" t="s">
         <v>183</v>
@@ -7197,8 +7197,8 @@
         <v>1039</v>
       </c>
       <c r="G76" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|File.OpenProject|RiderOpenSolution|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|File.OpenProject|RiderOpenSolution|CONTROL SHIFT O|</v>
       </c>
       <c r="H76" t="s">
         <v>186</v>
@@ -7225,8 +7225,8 @@
         <v>868</v>
       </c>
       <c r="G77" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Project Shortcut Keys|Project.Override|OverrideMethods|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Project Shortcut Keys|Project.Override|OverrideMethods|CONTROL ALT INSERT|</v>
       </c>
       <c r="H77" t="s">
         <v>195</v>
@@ -7253,8 +7253,8 @@
         <v>904</v>
       </c>
       <c r="G78" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.Find|Find|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Find|Find|CONTROL F|</v>
       </c>
       <c r="H78" t="s">
         <v>198</v>
@@ -7281,8 +7281,8 @@
         <v>905</v>
       </c>
       <c r="G79" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.FindinFiles|FindInPath|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindinFiles|FindInPath|CONTROL SHIFT F|</v>
       </c>
       <c r="H79" t="s">
         <v>201</v>
@@ -7309,8 +7309,8 @@
         <v>906</v>
       </c>
       <c r="G80" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.FindNext|FindNext|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindNext|FindNext|F3|</v>
       </c>
       <c r="H80" t="s">
         <v>204</v>
@@ -7334,8 +7334,8 @@
         <v>0</v>
       </c>
       <c r="G81" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.FindNextSelected||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindNextSelected||CONTROL F3|</v>
       </c>
       <c r="H81" t="s">
         <v>207</v>
@@ -7362,8 +7362,8 @@
         <v>907</v>
       </c>
       <c r="G82" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.FindPrevious|FindPrevious|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindPrevious|FindPrevious|SHIFT F3|</v>
       </c>
       <c r="H82" t="s">
         <v>210</v>
@@ -7387,8 +7387,8 @@
         <v>0</v>
       </c>
       <c r="G83" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.FindPreviousSelected||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.FindPreviousSelected||CONTROL SHIFT F3|</v>
       </c>
       <c r="H83" t="s">
         <v>213</v>
@@ -7415,8 +7415,8 @@
         <v>1178</v>
       </c>
       <c r="G84" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.GoToFindCombo|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.GoToFindCombo|N/A|CONTROL D|</v>
       </c>
       <c r="H84" t="s">
         <v>614</v>
@@ -7443,8 +7443,8 @@
         <v>1178</v>
       </c>
       <c r="G85" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.HiddenText|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.HiddenText|N/A|ALT F3, H|</v>
       </c>
       <c r="H85" t="s">
         <v>218</v>
@@ -7468,8 +7468,8 @@
         <v>0</v>
       </c>
       <c r="G86" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.IncrementalSearch||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.IncrementalSearch||CONTROL I|</v>
       </c>
       <c r="H86" t="s">
         <v>221</v>
@@ -7496,8 +7496,8 @@
         <v>1178</v>
       </c>
       <c r="G87" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.MatchCase|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.MatchCase|N/A|ALT F3, C|</v>
       </c>
       <c r="H87" t="s">
         <v>224</v>
@@ -7524,8 +7524,8 @@
         <v>1178</v>
       </c>
       <c r="G88" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.RegularExpression|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.RegularExpression|N/A|ALT F3, R|</v>
       </c>
       <c r="H88" t="s">
         <v>227</v>
@@ -7552,8 +7552,8 @@
         <v>912</v>
       </c>
       <c r="G89" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.Replace|Replace|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Replace|Replace|CONTROL H|</v>
       </c>
       <c r="H89" t="s">
         <v>230</v>
@@ -7580,8 +7580,8 @@
         <v>913</v>
       </c>
       <c r="G90" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.ReplaceinFiles|ReplaceInPath|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.ReplaceinFiles|ReplaceInPath|CONTROL SHIFT H|</v>
       </c>
       <c r="H90" t="s">
         <v>233</v>
@@ -7605,8 +7605,8 @@
         <v>0</v>
       </c>
       <c r="G91" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.ReverseIncrementalSearch||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.ReverseIncrementalSearch||CONTROL SHIFT I|</v>
       </c>
       <c r="H91" t="s">
         <v>236</v>
@@ -7633,8 +7633,8 @@
         <v>1178</v>
       </c>
       <c r="G92" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.StopSearch|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.StopSearch|N/A|ALT F3, S|</v>
       </c>
       <c r="H92" t="s">
         <v>239</v>
@@ -7661,8 +7661,8 @@
         <v>1178</v>
       </c>
       <c r="G93" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.Up|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Up|N/A|ALT F3, B|</v>
       </c>
       <c r="H93" t="s">
         <v>242</v>
@@ -7689,8 +7689,8 @@
         <v>1178</v>
       </c>
       <c r="G94" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.WholeWord|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.WholeWord|N/A|ALT F3, W|</v>
       </c>
       <c r="H94" t="s">
         <v>245</v>
@@ -7717,8 +7717,8 @@
         <v>1178</v>
       </c>
       <c r="G95" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Search and Replace Shortcut Keys|Edit.Wildcard|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Search and Replace Shortcut Keys|Edit.Wildcard|N/A|ALT F3, P|</v>
       </c>
       <c r="H95" t="s">
         <v>274</v>
@@ -7745,8 +7745,8 @@
         <v>629</v>
       </c>
       <c r="G96" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.BreakLine|EditorEnter|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.BreakLine|EditorEnter|ENTER || SHIFT ENTER|</v>
       </c>
       <c r="H96" t="s">
         <v>277</v>
@@ -7773,8 +7773,8 @@
         <v>974</v>
       </c>
       <c r="G97" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.CharTranspose|EditorTranspose|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CharTranspose|EditorTranspose|CONTROL T|</v>
       </c>
       <c r="H97" t="s">
         <v>280</v>
@@ -7798,8 +7798,8 @@
         <v>1</v>
       </c>
       <c r="G98" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.ClearBookmarks||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ClearBookmarks||CONTROL SHIFT F2 || CONTROL K, CONTROL L|</v>
       </c>
       <c r="H98" t="s">
         <v>283</v>
@@ -7823,8 +7823,8 @@
         <v>1</v>
       </c>
       <c r="G99" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.CollapsetoDefinitions||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CollapsetoDefinitions||CONTROL M, CONTROL O|</v>
       </c>
       <c r="H99" t="s">
         <v>286</v>
@@ -7851,8 +7851,8 @@
         <v>1219</v>
       </c>
       <c r="G100" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.CommentSelection|CommentByLineComment|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CommentSelection|CommentByLineComment|CONTROL K, CONTROL C|</v>
       </c>
       <c r="H100" t="s">
         <v>1493</v>
@@ -7879,8 +7879,8 @@
         <v>879</v>
       </c>
       <c r="G101" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.CompleteWord|CodeCompletion|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.CompleteWord|CodeCompletion|CONTROL SPACE || ALT RIGHT_ARROW|</v>
       </c>
       <c r="H101" t="s">
         <v>290</v>
@@ -7907,8 +7907,8 @@
         <v>603</v>
       </c>
       <c r="G102" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.Delete|$Delete|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.Delete|$Delete|DELETE|</v>
       </c>
       <c r="H102" t="s">
         <v>293</v>
@@ -7935,8 +7935,8 @@
         <v>632</v>
       </c>
       <c r="G103" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.DeleteBackwards|EditorBackSpace|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.DeleteBackwards|EditorBackSpace|BACKSPACE || SHIFT BACKSPACE|</v>
       </c>
       <c r="H103" t="s">
         <v>296</v>
@@ -7963,8 +7963,8 @@
         <v>1178</v>
       </c>
       <c r="G104" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.DeleteHorizontalWhiteSpace|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.DeleteHorizontalWhiteSpace|N/A|CONTROL K, CONTROL \|</v>
       </c>
       <c r="H104" t="s">
         <v>299</v>
@@ -7991,8 +7991,8 @@
         <v>1394</v>
       </c>
       <c r="G105" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.FormatDocument|ReformatCode|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.FormatDocument|ReformatCode|CONTROL K, CONTROL D|</v>
       </c>
       <c r="H105" t="s">
         <v>302</v>
@@ -8019,8 +8019,8 @@
         <v>1394</v>
       </c>
       <c r="G106" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.FormatSelection|ReformatCode|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.FormatSelection|ReformatCode|ALT F8 || CONTROL K, CONTROL F|</v>
       </c>
       <c r="H106" t="s">
         <v>305</v>
@@ -8047,8 +8047,8 @@
         <v>1178</v>
       </c>
       <c r="G107" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.HideSelection|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.HideSelection|N/A|CONTROL M, CONTROL H|</v>
       </c>
       <c r="H107" t="s">
         <v>308</v>
@@ -8075,9 +8075,9 @@
         <v>822</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
         <v>|Text Manipulation Shortcut Keys|Edit.InsertTab|EditorTab
-EditorIndentSelection|</v>
+EditorIndentSelection|TAB|</v>
       </c>
       <c r="H108" t="s">
         <v>311</v>
@@ -8104,8 +8104,8 @@
         <v>602</v>
       </c>
       <c r="G109" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.LineCut|EditorDeleteLine|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineCut|EditorDeleteLine|CONTROL L || SHIFT ALT L|</v>
       </c>
       <c r="H109" t="s">
         <v>314</v>
@@ -8132,8 +8132,8 @@
         <v>602</v>
       </c>
       <c r="G110" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.LineDelete|EditorDeleteLine|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineDelete|EditorDeleteLine|CONTROL SHIFT L|</v>
       </c>
       <c r="H110" t="s">
         <v>317</v>
@@ -8160,8 +8160,8 @@
         <v>634</v>
       </c>
       <c r="G111" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.LineOpenAbove|EditorStartNewLineBefore|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineOpenAbove|EditorStartNewLineBefore|CONTROL ENTER|</v>
       </c>
       <c r="H111" t="s">
         <v>320</v>
@@ -8188,8 +8188,8 @@
         <v>633</v>
       </c>
       <c r="G112" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.LineOpenBelow|EditorStartNewLine|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineOpenBelow|EditorStartNewLine|CONTROL SHIFT ENTER|</v>
       </c>
       <c r="H112" t="s">
         <v>323</v>
@@ -8213,8 +8213,8 @@
         <v>0</v>
       </c>
       <c r="G113" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.LineTranspose||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.LineTranspose||SHIFT ALT T|</v>
       </c>
       <c r="H113" t="s">
         <v>326</v>
@@ -8241,8 +8241,8 @@
         <v>874</v>
       </c>
       <c r="G114" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.MakeLowercase|EditorToggleCase|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.MakeLowercase|EditorToggleCase|CONTROL U|</v>
       </c>
       <c r="H114" t="s">
         <v>329</v>
@@ -8269,8 +8269,8 @@
         <v>874</v>
       </c>
       <c r="G115" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.MakeUppercase|EditorToggleCase|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.MakeUppercase|EditorToggleCase|CONTROL SHIFT U|</v>
       </c>
       <c r="H115" t="s">
         <v>332</v>
@@ -8297,8 +8297,8 @@
         <v>631</v>
       </c>
       <c r="G116" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.OvertypeMode|EditorToggleInsertState|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.OvertypeMode|EditorToggleInsertState|INSERT|</v>
       </c>
       <c r="H116" t="s">
         <v>335</v>
@@ -8322,8 +8322,8 @@
         <v>1</v>
       </c>
       <c r="G117" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.StopHidingCurrent||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.StopHidingCurrent||CONTROL M, CONTROL U|</v>
       </c>
       <c r="H117" t="s">
         <v>338</v>
@@ -8347,8 +8347,8 @@
         <v>1</v>
       </c>
       <c r="G118" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.StopOutlining||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.StopOutlining||CONTROL M, CONTROL P|</v>
       </c>
       <c r="H118" t="s">
         <v>341</v>
@@ -8372,8 +8372,8 @@
         <v>1</v>
       </c>
       <c r="G119" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.SwapAnchor||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.SwapAnchor||CONTROL R, CONTROL P|</v>
       </c>
       <c r="H119" t="s">
         <v>344</v>
@@ -8400,8 +8400,8 @@
         <v>630</v>
       </c>
       <c r="G120" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.TabLeft|EditorUnindentSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.TabLeft|EditorUnindentSelection|SHIFT TAB|</v>
       </c>
       <c r="H120" t="s">
         <v>347</v>
@@ -8428,9 +8428,9 @@
         <v>1494</v>
       </c>
       <c r="G121" s="1" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
         <v>|Text Manipulation Shortcut Keys|Edit.ToggleAllOutlining|CollapseAll
-ExpandAll|</v>
+ExpandAll|CONTROL M, CONTROL L|</v>
       </c>
       <c r="H121" t="s">
         <v>350</v>
@@ -8457,8 +8457,8 @@
         <v>628</v>
       </c>
       <c r="G122" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.ToggleBookmark|ToggleBookmark|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleBookmark|ToggleBookmark|CONTROL F2 || CONTROL K, CONTROL K|</v>
       </c>
       <c r="H122" t="s">
         <v>353</v>
@@ -8482,8 +8482,8 @@
         <v>1</v>
       </c>
       <c r="G123" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.ToggleOutliningExpansion||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleOutliningExpansion||CONTROL M, CONTROL M|</v>
       </c>
       <c r="H123" t="s">
         <v>356</v>
@@ -8510,8 +8510,8 @@
         <v>1178</v>
       </c>
       <c r="G124" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.ToggleTaskListShortcut|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleTaskListShortcut|N/A|CONTROL K, CONTROL H|</v>
       </c>
       <c r="H124" t="s">
         <v>359</v>
@@ -8538,8 +8538,8 @@
         <v>1002</v>
       </c>
       <c r="G125" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.ToggleWordWrap|EditorToggleUseSoftWraps|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ToggleWordWrap|EditorToggleUseSoftWraps|CONTROL R, CONTROL R|</v>
       </c>
       <c r="H125" t="s">
         <v>362</v>
@@ -8566,8 +8566,8 @@
         <v>1219</v>
       </c>
       <c r="G126" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.UnCommentSelection|CommentByLineComment|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.UnCommentSelection|CommentByLineComment|CONTROL K, CONTROL U|</v>
       </c>
       <c r="H126" t="s">
         <v>617</v>
@@ -8594,8 +8594,8 @@
         <v>1001</v>
       </c>
       <c r="G127" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.ViewWhiteSpace|EditorToggleShowWhitespaces|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.ViewWhiteSpace|EditorToggleShowWhitespaces|CONTROL SHIFT 8 || CONTROL R, CONTROL W|</v>
       </c>
       <c r="H127" t="s">
         <v>366</v>
@@ -8622,8 +8622,8 @@
         <v>876</v>
       </c>
       <c r="G128" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.WordDeleteToEnd|EditorDeleteToWordEnd|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.WordDeleteToEnd|EditorDeleteToWordEnd|CONTROL DELETE|</v>
       </c>
       <c r="H128" t="s">
         <v>369</v>
@@ -8650,8 +8650,8 @@
         <v>875</v>
       </c>
       <c r="G129" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.WordDeleteToStart|EditorDeleteToWordStart|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.WordDeleteToStart|EditorDeleteToWordStart|CONTROL BACKSPACE|</v>
       </c>
       <c r="H129" t="s">
         <v>372</v>
@@ -8678,8 +8678,8 @@
         <v>1178</v>
       </c>
       <c r="G130" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Manipulation Shortcut Keys|Edit.WordTranspose|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Manipulation Shortcut Keys|Edit.WordTranspose|N/A|CONTROL SHIFT T|</v>
       </c>
       <c r="H130" t="s">
         <v>375</v>
@@ -8706,8 +8706,8 @@
         <v>818</v>
       </c>
       <c r="G131" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.CharLeft|EditorLeft|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.CharLeft|EditorLeft|LEFT_ARROW|</v>
       </c>
       <c r="H131" t="s">
         <v>379</v>
@@ -8734,8 +8734,8 @@
         <v>819</v>
       </c>
       <c r="G132" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.CharRight|EditorRight|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.CharRight|EditorRight|RIGHT_ARROW|</v>
       </c>
       <c r="H132" t="s">
         <v>382</v>
@@ -8762,8 +8762,8 @@
         <v>883</v>
       </c>
       <c r="G133" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.DocumentEnd|EditorTextEnd|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.DocumentEnd|EditorTextEnd|CONTROL END|</v>
       </c>
       <c r="H133" t="s">
         <v>385</v>
@@ -8790,8 +8790,8 @@
         <v>884</v>
       </c>
       <c r="G134" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.DocumentStart|EditorTextStart|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.DocumentStart|EditorTextStart|CONTROL HOME|</v>
       </c>
       <c r="H134" t="s">
         <v>388</v>
@@ -8818,8 +8818,8 @@
         <v>873</v>
       </c>
       <c r="G135" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.GoTo|GotoLine|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.GoTo|GotoLine|CONTROL G|</v>
       </c>
       <c r="H135" t="s">
         <v>391</v>
@@ -8846,8 +8846,8 @@
         <v>1178</v>
       </c>
       <c r="G136" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.GotoBrace|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.GotoBrace|N/A|CONTROL ]|</v>
       </c>
       <c r="H136" t="s">
         <v>394</v>
@@ -8874,8 +8874,8 @@
         <v>877</v>
       </c>
       <c r="G137" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.LineDown|EditorDown|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineDown|EditorDown|DOWN_ARROW|</v>
       </c>
       <c r="H137" t="s">
         <v>397</v>
@@ -8902,8 +8902,8 @@
         <v>636</v>
       </c>
       <c r="G138" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.LineEnd|EditorLineEnd|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineEnd|EditorLineEnd|END|</v>
       </c>
       <c r="H138" t="s">
         <v>400</v>
@@ -8930,8 +8930,8 @@
         <v>635</v>
       </c>
       <c r="G139" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.LineStart|EditorLineStart|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineStart|EditorLineStart|HOME|</v>
       </c>
       <c r="H139" t="s">
         <v>403</v>
@@ -8958,8 +8958,8 @@
         <v>878</v>
       </c>
       <c r="G140" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.LineUp|EditorUp|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.LineUp|EditorUp|UP_ARROW|</v>
       </c>
       <c r="H140" t="s">
         <v>406</v>
@@ -8986,8 +8986,8 @@
         <v>863</v>
       </c>
       <c r="G141" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.NextBookmark|GotoNextBookmark|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.NextBookmark|GotoNextBookmark|F2 || CONTROL K, CONTROL N|</v>
       </c>
       <c r="H141" t="s">
         <v>409</v>
@@ -9014,8 +9014,8 @@
         <v>821</v>
       </c>
       <c r="G142" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.PageDown|EditorPageDown|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.PageDown|EditorPageDown|PAGE_DOWN|</v>
       </c>
       <c r="H142" t="s">
         <v>412</v>
@@ -9042,8 +9042,8 @@
         <v>820</v>
       </c>
       <c r="G143" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.PageUp|EditorPageUp|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.PageUp|EditorPageUp|PAGE_UP|</v>
       </c>
       <c r="H143" t="s">
         <v>415</v>
@@ -9070,8 +9070,8 @@
         <v>864</v>
       </c>
       <c r="G144" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.PreviousBookmark|GotoPreviousBookmark|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.PreviousBookmark|GotoPreviousBookmark|SHIFT F2 || CONTROL K, CONTROL P|</v>
       </c>
       <c r="H144" t="s">
         <v>418</v>
@@ -9098,8 +9098,8 @@
         <v>1178</v>
       </c>
       <c r="G145" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.QuickInfo|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.QuickInfo|N/A|CONTROL K, CONTROL I|</v>
       </c>
       <c r="H145" t="s">
         <v>421</v>
@@ -9126,8 +9126,8 @@
         <v>902</v>
       </c>
       <c r="G146" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.ScrollLineDown|EditorScrollDown|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.ScrollLineDown|EditorScrollDown|CONTROL DOWN_ARROW|</v>
       </c>
       <c r="H146" t="s">
         <v>424</v>
@@ -9154,8 +9154,8 @@
         <v>903</v>
       </c>
       <c r="G147" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.ScrollLineUp|EditorScrollUp|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.ScrollLineUp|EditorScrollUp|CONTROL UP_ARROW|</v>
       </c>
       <c r="H147" t="s">
         <v>427</v>
@@ -9179,8 +9179,8 @@
         <v>0</v>
       </c>
       <c r="G148" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.ShowTileGrid||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.ShowTileGrid||CONTROL SHIFT G|</v>
       </c>
       <c r="H148" t="s">
         <v>430</v>
@@ -9207,8 +9207,8 @@
         <v>892</v>
       </c>
       <c r="G149" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.WordNext|EditorNextWord|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.WordNext|EditorNextWord|CONTROL RIGHT_ARROW|</v>
       </c>
       <c r="H149" t="s">
         <v>433</v>
@@ -9235,8 +9235,8 @@
         <v>891</v>
       </c>
       <c r="G150" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|Edit.WordPrevious|EditorPreviousWord|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|Edit.WordPrevious|EditorPreviousWord|CONTROL LEFT_ARROW|</v>
       </c>
       <c r="H150" t="s">
         <v>436</v>
@@ -9261,8 +9261,8 @@
       </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|View.BrowseNext||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|View.BrowseNext||CONTROL num+ || CONTROL SHIFT 1|</v>
       </c>
       <c r="H151" t="s">
         <v>438</v>
@@ -9287,8 +9287,8 @@
       </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Navigation Shortcut Keys|View.BrowsePrevious||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Navigation Shortcut Keys|View.BrowsePrevious||CONTROL num– || CONTROL SHIFT 2|</v>
       </c>
       <c r="H152" t="s">
         <v>440</v>
@@ -9315,8 +9315,8 @@
         <v>880</v>
       </c>
       <c r="G153" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.CharLeftExtend|EditorLeftWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharLeftExtend|EditorLeftWithSelection|SHIFT LEFT_ARROW|</v>
       </c>
       <c r="H153" t="s">
         <v>446</v>
@@ -9340,8 +9340,8 @@
         <v>0</v>
       </c>
       <c r="G154" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.CharLeftExtendColumn||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharLeftExtendColumn||SHIFT ALT LEFT_ARROW|</v>
       </c>
       <c r="H154" t="s">
         <v>449</v>
@@ -9368,8 +9368,8 @@
         <v>881</v>
       </c>
       <c r="G155" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.CharRightExtend|EditorRightWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharRightExtend|EditorRightWithSelection|SHIFT RIGHT_ARROW|</v>
       </c>
       <c r="H155" t="s">
         <v>452</v>
@@ -9393,8 +9393,8 @@
         <v>0</v>
       </c>
       <c r="G156" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.CharRightExtendColumn||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.CharRightExtendColumn||SHIFT ALT RIGHT_ARROW|</v>
       </c>
       <c r="H156" t="s">
         <v>455</v>
@@ -9421,8 +9421,8 @@
         <v>885</v>
       </c>
       <c r="G157" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.DocumentEndExtend|EditorTextEndWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.DocumentEndExtend|EditorTextEndWithSelection|CONTROL SHIFT END|</v>
       </c>
       <c r="H157" t="s">
         <v>458</v>
@@ -9449,8 +9449,8 @@
         <v>886</v>
       </c>
       <c r="G158" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.DocumentStartExtend|EditorTextStartWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.DocumentStartExtend|EditorTextStartWithSelection|CONTROL SHIFT HOME|</v>
       </c>
       <c r="H158" t="s">
         <v>461</v>
@@ -9474,8 +9474,8 @@
         <v>0</v>
       </c>
       <c r="G159" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.GotoBraceExtend||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.GotoBraceExtend||CONTROL SHIFT ]|</v>
       </c>
       <c r="H159" t="s">
         <v>464</v>
@@ -9502,8 +9502,8 @@
         <v>882</v>
       </c>
       <c r="G160" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineDownExtend|EditorDownWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineDownExtend|EditorDownWithSelection|SHIFT DOWN_ARROW|</v>
       </c>
       <c r="H160" t="s">
         <v>467</v>
@@ -9530,8 +9530,8 @@
         <v>909</v>
       </c>
       <c r="G161" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineDownExtendColumn|MoveLineDown|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineDownExtendColumn|MoveLineDown|SHIFT ALT DOWN_ARROW|</v>
       </c>
       <c r="H161" t="s">
         <v>470</v>
@@ -9558,8 +9558,8 @@
         <v>887</v>
       </c>
       <c r="G162" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineEndExtend|EditorLineEndWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineEndExtend|EditorLineEndWithSelection|SHIFT END|</v>
       </c>
       <c r="H162" t="s">
         <v>473</v>
@@ -9583,8 +9583,8 @@
         <v>0</v>
       </c>
       <c r="G163" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineEndExtendColumn||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineEndExtendColumn||SHIFT ALT END|</v>
       </c>
       <c r="H163" t="s">
         <v>476</v>
@@ -9611,8 +9611,8 @@
         <v>888</v>
       </c>
       <c r="G164" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineStartExtend|EditorLineStartWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineStartExtend|EditorLineStartWithSelection|SHIFT HOME|</v>
       </c>
       <c r="H164" t="s">
         <v>479</v>
@@ -9636,8 +9636,8 @@
         <v>0</v>
       </c>
       <c r="G165" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineStartExtendColumn||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineStartExtendColumn||SHIFT ALT HOME|</v>
       </c>
       <c r="H165" t="s">
         <v>482</v>
@@ -9664,8 +9664,8 @@
         <v>901</v>
       </c>
       <c r="G166" s="1" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineUpExtend|EditorUpWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineUpExtend|EditorUpWithSelection|SHIFT UP_ARROW|</v>
       </c>
       <c r="H166" t="s">
         <v>484</v>
@@ -9692,8 +9692,8 @@
         <v>908</v>
       </c>
       <c r="G167" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.LineUpExtendColumn|MoveLineUp|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.LineUpExtendColumn|MoveLineUp|SHIFT ALT UP_ARROW|</v>
       </c>
       <c r="H167" t="s">
         <v>487</v>
@@ -9720,8 +9720,8 @@
         <v>897</v>
       </c>
       <c r="G168" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.PageDownExtend|EditorPageDownWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.PageDownExtend|EditorPageDownWithSelection|SHIFT PAGE_DOWN|</v>
       </c>
       <c r="H168" t="s">
         <v>490</v>
@@ -9748,8 +9748,8 @@
         <v>898</v>
       </c>
       <c r="G169" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.PageUpExtend|EditorPageUpWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.PageUpExtend|EditorPageUpWithSelection|SHIFT PAGE_UP|</v>
       </c>
       <c r="H169" t="s">
         <v>493</v>
@@ -9776,8 +9776,8 @@
         <v>627</v>
       </c>
       <c r="G170" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.SelectAll|$SelectAll|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.SelectAll|$SelectAll|CONTROL A|</v>
       </c>
       <c r="H170" t="s">
         <v>496</v>
@@ -9804,8 +9804,8 @@
         <v>1179</v>
       </c>
       <c r="G171" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.SelectCurrentWord|EditorSelectWord|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.SelectCurrentWord|EditorSelectWord|CONTROL W|</v>
       </c>
       <c r="H171" t="s">
         <v>499</v>
@@ -9832,8 +9832,8 @@
         <v>1178</v>
       </c>
       <c r="G172" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.SelectToLastGoBack|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.SelectToLastGoBack|N/A|CONTROL =|</v>
       </c>
       <c r="H172" t="s">
         <v>502</v>
@@ -9860,8 +9860,8 @@
         <v>896</v>
       </c>
       <c r="G173" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.ViewBottomExtend|EditorMoveToPageBottomWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.ViewBottomExtend|EditorMoveToPageBottomWithSelection|CONTROL SHIFT PAGE_DOWN|</v>
       </c>
       <c r="H173" t="s">
         <v>505</v>
@@ -9888,8 +9888,8 @@
         <v>895</v>
       </c>
       <c r="G174" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.ViewTopExtend|EditorMoveToPageTopWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.ViewTopExtend|EditorMoveToPageTopWithSelection|CONTROL SHIFT PAGE_UP|</v>
       </c>
       <c r="H174" t="s">
         <v>508</v>
@@ -9916,8 +9916,8 @@
         <v>894</v>
       </c>
       <c r="G175" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.WordNextExtend|EditorNextWordWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordNextExtend|EditorNextWordWithSelection|CONTROL SHIFT RIGHT_ARROW|</v>
       </c>
       <c r="H175" t="s">
         <v>511</v>
@@ -9944,8 +9944,8 @@
         <v>911</v>
       </c>
       <c r="G176" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.WordNextExtendColumn|MoveElementRight|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordNextExtendColumn|MoveElementRight|CONTROL SHIFT ALT RIGHT_ARROW|</v>
       </c>
       <c r="H176" t="s">
         <v>514</v>
@@ -9972,8 +9972,8 @@
         <v>893</v>
       </c>
       <c r="G177" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.WordPreviousExtend|EditorPreviousWordWithSelection|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordPreviousExtend|EditorPreviousWordWithSelection|CONTROL SHIFT LEFT_ARROW|</v>
       </c>
       <c r="H177" t="s">
         <v>517</v>
@@ -10000,8 +10000,8 @@
         <v>910</v>
       </c>
       <c r="G178" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Text Selection Shortcut Keys|Edit.WordPreviousExtendColumn|MoveElementLeft|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Text Selection Shortcut Keys|Edit.WordPreviousExtendColumn|MoveElementLeft|CONTROL SHIFT ALT LEFT_ARROW|</v>
       </c>
       <c r="H178" t="s">
         <v>520</v>
@@ -10025,8 +10025,8 @@
         <v>0</v>
       </c>
       <c r="G179" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|Tools.CommandWindowMarkMode||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|Tools.CommandWindowMarkMode||CONTROL SHIFT M|</v>
       </c>
       <c r="H179" t="s">
         <v>609</v>
@@ -10053,8 +10053,8 @@
         <v>832</v>
       </c>
       <c r="G180" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.ClassView|ActivateHierarchyToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.ClassView|ActivateHierarchyToolWindow|CONTROL SHIFT C|</v>
       </c>
       <c r="H180" t="s">
         <v>525</v>
@@ -10081,8 +10081,8 @@
         <v>840</v>
       </c>
       <c r="G181" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.CommandWindow|IdeScriptingConsole|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.CommandWindow|IdeScriptingConsole|CONTROL ALT A|</v>
       </c>
       <c r="H181" t="s">
         <v>619</v>
@@ -10109,8 +10109,8 @@
         <v>827</v>
       </c>
       <c r="G182" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.DocumentOutline|ActivateStructureToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.DocumentOutline|ActivateStructureToolWindow|CONTROL ALT D|</v>
       </c>
       <c r="H182" t="s">
         <v>529</v>
@@ -10137,8 +10137,8 @@
         <v>826</v>
       </c>
       <c r="G183" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.Favorites|ActivateFavoritesToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.Favorites|ActivateFavoritesToolWindow|CONTROL ALT F|</v>
       </c>
       <c r="H183" t="s">
         <v>550</v>
@@ -10165,8 +10165,8 @@
         <v>828</v>
       </c>
       <c r="G184" s="1" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.Output|ActivateRunToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.Output|ActivateRunToolWindow|ALT 2 || CONTROL ALT O|</v>
       </c>
       <c r="H184" t="s">
         <v>533</v>
@@ -10193,8 +10193,8 @@
         <v>1178</v>
       </c>
       <c r="G185" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.PropertiesWindow|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.PropertiesWindow|N/A|ALT ENTER|</v>
       </c>
       <c r="H185" t="s">
         <v>536</v>
@@ -10218,8 +10218,8 @@
         <v>0</v>
       </c>
       <c r="G186" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.ResourceView||</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.ResourceView||CONTROL SHIFT E|</v>
       </c>
       <c r="H186" t="s">
         <v>539</v>
@@ -10246,8 +10246,8 @@
         <v>842</v>
       </c>
       <c r="G187" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.ServerExplorer|ActivateDatabaseToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.ServerExplorer|ActivateDatabaseToolWindow|CONTROL ALT S|</v>
       </c>
       <c r="H187" t="s">
         <v>542</v>
@@ -10274,8 +10274,8 @@
         <v>833</v>
       </c>
       <c r="G188" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.SolutionExplorer|ActivateProjectToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.SolutionExplorer|ActivateProjectToolWindow|CONTROL ALT L|</v>
       </c>
       <c r="H188" t="s">
         <v>551</v>
@@ -10302,8 +10302,8 @@
         <v>841</v>
       </c>
       <c r="G189" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.TaskList|ActivateTODOToolWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.TaskList|ActivateTODOToolWindow|CONTROL ALT K|</v>
       </c>
       <c r="H189" t="s">
         <v>620</v>
@@ -10330,8 +10330,8 @@
         <v>1178</v>
       </c>
       <c r="G190" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Tool Window Shortcut Keys|View.Toolbox|N/A|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Tool Window Shortcut Keys|View.Toolbox|N/A|CONTROL ALT X|</v>
       </c>
       <c r="H190" t="s">
         <v>549</v>
@@ -10358,8 +10358,8 @@
         <v>843</v>
       </c>
       <c r="G191" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|View.FullScreen|ToggleFullScreen|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|View.FullScreen|ToggleFullScreen|SHIFT ALT ENTER|</v>
       </c>
       <c r="H191" t="s">
         <v>556</v>
@@ -10386,8 +10386,8 @@
         <v>830</v>
       </c>
       <c r="G192" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|View.NavigateBackward|Back|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|View.NavigateBackward|Back|CONTROL -|</v>
       </c>
       <c r="H192" t="s">
         <v>559</v>
@@ -10414,8 +10414,8 @@
         <v>831</v>
       </c>
       <c r="G193" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|View.NavigateForward|Forward|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|View.NavigateForward|Forward|CONTROL SHIFT -|</v>
       </c>
       <c r="H193" t="s">
         <v>562</v>
@@ -10442,8 +10442,8 @@
         <v>834</v>
       </c>
       <c r="G194" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.ActivateDocumentWindow|FocusEditor|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.ActivateDocumentWindow|FocusEditor|ESC || ALT 0|</v>
       </c>
       <c r="H194" t="s">
         <v>29</v>
@@ -10470,8 +10470,8 @@
         <v>845</v>
       </c>
       <c r="G195" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.CloseDocumentWindow|CloseContent|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.CloseDocumentWindow|CloseContent|CONTROL F4|</v>
       </c>
       <c r="H195" t="s">
         <v>567</v>
@@ -10498,8 +10498,8 @@
         <v>844</v>
       </c>
       <c r="G196" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.CloseToolWindow|HideActiveWindow|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.CloseToolWindow|HideActiveWindow|SHIFT ESC|</v>
       </c>
       <c r="H196" t="s">
         <v>570</v>
@@ -10526,8 +10526,8 @@
         <v>848</v>
       </c>
       <c r="G197" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.NextDocumentWindow|NextTab|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextDocumentWindow|NextTab|CONTROL F6 || CONTROL TAB|</v>
       </c>
       <c r="H197" t="s">
         <v>573</v>
@@ -10554,8 +10554,8 @@
         <v>846</v>
       </c>
       <c r="G198" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.NextPane|NextSplitter|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextPane|NextSplitter|ALT F6|</v>
       </c>
       <c r="H198" t="s">
         <v>576</v>
@@ -10582,8 +10582,8 @@
         <v>846</v>
       </c>
       <c r="G199" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.NextSplitPane|NextSplitter|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextSplitPane|NextSplitter|F6|</v>
       </c>
       <c r="H199" t="s">
         <v>579</v>
@@ -10610,8 +10610,8 @@
         <v>848</v>
       </c>
       <c r="G200" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.NextTab|NextTab|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.NextTab|NextTab|CONTROL PAGE_DOWN|</v>
       </c>
       <c r="H200" t="s">
         <v>582</v>
@@ -10638,8 +10638,8 @@
         <v>849</v>
       </c>
       <c r="G201" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.PreviousDocumentWindow|PreviousTab|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousDocumentWindow|PreviousTab|CONTROL SHIFT F6 || CONTROL SHIFT TAB|</v>
       </c>
       <c r="H201" t="s">
         <v>585</v>
@@ -10666,8 +10666,8 @@
         <v>847</v>
       </c>
       <c r="G202" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.PreviousPane|PrevSplitter|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousPane|PrevSplitter|SHIFT ALT F6|</v>
       </c>
       <c r="H202" t="s">
         <v>588</v>
@@ -10694,8 +10694,8 @@
         <v>847</v>
       </c>
       <c r="G203" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.PreviousSplitPane|PrevSplitter|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousSplitPane|PrevSplitter|SHIFT F6|</v>
       </c>
       <c r="H203" t="s">
         <v>591</v>
@@ -10722,8 +10722,8 @@
         <v>849</v>
       </c>
       <c r="G204" t="str">
-        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"</f>
-        <v>|Window Management Shortcut Keys|Window.PreviousTab|PreviousTab|</v>
+        <f>"|" &amp; Table1[[#This Row],[VC_Command_Class]] &amp; "|" &amp;Table1[[#This Row],[VC_Command_Name]] &amp; "|" &amp;Table1[[#This Row],[IDEA_Keymap_ID]] &amp; "|"&amp; Table1[[#This Row],[VC_Shortcut_Keys]]&amp; "|"</f>
+        <v>|Window Management Shortcut Keys|Window.PreviousTab|PreviousTab|CONTROL PAGE_UP|</v>
       </c>
       <c r="H204" t="s">
         <v>594</v>

</xml_diff>